<commit_message>
data up to 12
</commit_message>
<xml_diff>
--- a/fb-survey-communityState.xlsx
+++ b/fb-survey-communityState.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="185">
   <si>
     <t>Alaska</t>
   </si>
@@ -548,6 +548,27 @@
   </si>
   <si>
     <t>01 06 2020</t>
+  </si>
+  <si>
+    <t>02 06 2020</t>
+  </si>
+  <si>
+    <t>03 06 2020</t>
+  </si>
+  <si>
+    <t>04 06 2020</t>
+  </si>
+  <si>
+    <t>05 06 2020</t>
+  </si>
+  <si>
+    <t>06 06 2020</t>
+  </si>
+  <si>
+    <t>07 06 2020</t>
+  </si>
+  <si>
+    <t>08 06 2020</t>
   </si>
 </sst>
 </file>
@@ -879,7 +900,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BE123"/>
+  <dimension ref="A1:BE130"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -8260,7 +8281,7 @@
         <v>11.746748</v>
       </c>
       <c r="M119">
-        <v>16.3875723</v>
+        <v>16.3863843</v>
       </c>
       <c r="O119">
         <v>8.580508500000001</v>
@@ -8421,7 +8442,7 @@
         <v>11.9238268</v>
       </c>
       <c r="M120">
-        <v>16.5559284</v>
+        <v>16.5547062</v>
       </c>
       <c r="O120">
         <v>8.709143600000001</v>
@@ -8582,7 +8603,7 @@
         <v>11.7097194</v>
       </c>
       <c r="M121">
-        <v>16.5502948</v>
+        <v>16.5490652</v>
       </c>
       <c r="O121">
         <v>9.4717293</v>
@@ -8722,13 +8743,13 @@
         <v>16.8883273</v>
       </c>
       <c r="F122">
-        <v>14.9010826</v>
+        <v>14.899868</v>
       </c>
       <c r="G122">
-        <v>11.3636146</v>
+        <v>11.3613703</v>
       </c>
       <c r="H122">
-        <v>15.8172606</v>
+        <v>15.8248666</v>
       </c>
       <c r="I122">
         <v>16.3292514</v>
@@ -8740,10 +8761,10 @@
         <v>14.9725777</v>
       </c>
       <c r="L122">
-        <v>11.698427</v>
+        <v>11.7010078</v>
       </c>
       <c r="M122">
-        <v>16.2645222</v>
+        <v>16.2632995</v>
       </c>
       <c r="O122">
         <v>8.447979399999999</v>
@@ -8761,7 +8782,7 @@
         <v>18.7807983</v>
       </c>
       <c r="T122">
-        <v>14.8358424</v>
+        <v>14.8334356</v>
       </c>
       <c r="U122">
         <v>15.4003321</v>
@@ -8818,7 +8839,7 @@
         <v>15.7410436</v>
       </c>
       <c r="AN122">
-        <v>14.6708435</v>
+        <v>14.6682243</v>
       </c>
       <c r="AO122">
         <v>14.4169342</v>
@@ -8842,10 +8863,10 @@
         <v>20.3004927</v>
       </c>
       <c r="AV122">
-        <v>13.9536008</v>
+        <v>13.9523877</v>
       </c>
       <c r="AW122">
-        <v>14.669349</v>
+        <v>14.6713623</v>
       </c>
       <c r="AX122">
         <v>16.4394038</v>
@@ -8857,7 +8878,7 @@
         <v>9.8931817</v>
       </c>
       <c r="BB122">
-        <v>13.4345321</v>
+        <v>13.4325572</v>
       </c>
       <c r="BC122">
         <v>14.4930411</v>
@@ -8872,6 +8893,974 @@
     <row r="123" spans="1:57">
       <c r="A123" t="s">
         <v>177</v>
+      </c>
+      <c r="B123">
+        <v>12.5605164</v>
+      </c>
+      <c r="C123">
+        <v>18.7590793</v>
+      </c>
+      <c r="D123">
+        <v>16.7497956</v>
+      </c>
+      <c r="F123">
+        <v>14.9050471</v>
+      </c>
+      <c r="G123">
+        <v>11.3592035</v>
+      </c>
+      <c r="H123">
+        <v>15.5485981</v>
+      </c>
+      <c r="I123">
+        <v>15.9224559</v>
+      </c>
+      <c r="J123">
+        <v>15.546697</v>
+      </c>
+      <c r="K123">
+        <v>14.5731478</v>
+      </c>
+      <c r="L123">
+        <v>11.8885942</v>
+      </c>
+      <c r="M123">
+        <v>16.1794707</v>
+      </c>
+      <c r="O123">
+        <v>8.8235294</v>
+      </c>
+      <c r="P123">
+        <v>21.6181246</v>
+      </c>
+      <c r="Q123">
+        <v>13.4141061</v>
+      </c>
+      <c r="R123">
+        <v>16.1735404</v>
+      </c>
+      <c r="S123">
+        <v>18.9726432</v>
+      </c>
+      <c r="T123">
+        <v>14.6231776</v>
+      </c>
+      <c r="U123">
+        <v>15.4351575</v>
+      </c>
+      <c r="V123">
+        <v>19.0531787</v>
+      </c>
+      <c r="W123">
+        <v>17.3041009</v>
+      </c>
+      <c r="X123">
+        <v>15.7569205</v>
+      </c>
+      <c r="Y123">
+        <v>10.0152572</v>
+      </c>
+      <c r="Z123">
+        <v>14.1996381</v>
+      </c>
+      <c r="AA123">
+        <v>17.5769097</v>
+      </c>
+      <c r="AB123">
+        <v>14.81863</v>
+      </c>
+      <c r="AD123">
+        <v>19.7109308</v>
+      </c>
+      <c r="AE123">
+        <v>9.2229922</v>
+      </c>
+      <c r="AF123">
+        <v>13.9046305</v>
+      </c>
+      <c r="AG123">
+        <v>17.8383689</v>
+      </c>
+      <c r="AH123">
+        <v>21.426789</v>
+      </c>
+      <c r="AI123">
+        <v>13.4365526</v>
+      </c>
+      <c r="AJ123">
+        <v>17.5675617</v>
+      </c>
+      <c r="AK123">
+        <v>14.1010263</v>
+      </c>
+      <c r="AL123">
+        <v>12.1167964</v>
+      </c>
+      <c r="AM123">
+        <v>15.5392094</v>
+      </c>
+      <c r="AN123">
+        <v>14.3210989</v>
+      </c>
+      <c r="AO123">
+        <v>14.1231491</v>
+      </c>
+      <c r="AP123">
+        <v>11.5758286</v>
+      </c>
+      <c r="AQ123">
+        <v>12.3378264</v>
+      </c>
+      <c r="AR123">
+        <v>7.9882485</v>
+      </c>
+      <c r="AS123">
+        <v>15.3034019</v>
+      </c>
+      <c r="AT123">
+        <v>14.2592257</v>
+      </c>
+      <c r="AU123">
+        <v>20.4802587</v>
+      </c>
+      <c r="AV123">
+        <v>13.7841213</v>
+      </c>
+      <c r="AW123">
+        <v>14.4293391</v>
+      </c>
+      <c r="AX123">
+        <v>16.3772043</v>
+      </c>
+      <c r="AY123">
+        <v>15.2842832</v>
+      </c>
+      <c r="BA123">
+        <v>9.915507</v>
+      </c>
+      <c r="BB123">
+        <v>13.3723583</v>
+      </c>
+      <c r="BC123">
+        <v>14.4291145</v>
+      </c>
+      <c r="BD123">
+        <v>13.6497005</v>
+      </c>
+      <c r="BE123">
+        <v>15.5304343</v>
+      </c>
+    </row>
+    <row r="124" spans="1:57">
+      <c r="A124" t="s">
+        <v>178</v>
+      </c>
+      <c r="B124">
+        <v>12.3400853</v>
+      </c>
+      <c r="C124">
+        <v>18.6678701</v>
+      </c>
+      <c r="D124">
+        <v>17.4503912</v>
+      </c>
+      <c r="F124">
+        <v>15.1337443</v>
+      </c>
+      <c r="G124">
+        <v>11.5093612</v>
+      </c>
+      <c r="H124">
+        <v>15.2753969</v>
+      </c>
+      <c r="I124">
+        <v>15.5308322</v>
+      </c>
+      <c r="J124">
+        <v>16.277713</v>
+      </c>
+      <c r="K124">
+        <v>14.8768283</v>
+      </c>
+      <c r="L124">
+        <v>11.7416337</v>
+      </c>
+      <c r="M124">
+        <v>15.8710085</v>
+      </c>
+      <c r="O124">
+        <v>8.6385179</v>
+      </c>
+      <c r="P124">
+        <v>21.4670109</v>
+      </c>
+      <c r="Q124">
+        <v>13.1892586</v>
+      </c>
+      <c r="R124">
+        <v>16.0778909</v>
+      </c>
+      <c r="S124">
+        <v>18.7495091</v>
+      </c>
+      <c r="T124">
+        <v>15.0236843</v>
+      </c>
+      <c r="U124">
+        <v>15.0369839</v>
+      </c>
+      <c r="V124">
+        <v>19.3939806</v>
+      </c>
+      <c r="W124">
+        <v>16.8338189</v>
+      </c>
+      <c r="X124">
+        <v>15.8282473</v>
+      </c>
+      <c r="Y124">
+        <v>10.4820628</v>
+      </c>
+      <c r="Z124">
+        <v>14.0770636</v>
+      </c>
+      <c r="AA124">
+        <v>17.6398343</v>
+      </c>
+      <c r="AB124">
+        <v>14.9537741</v>
+      </c>
+      <c r="AD124">
+        <v>19.9505473</v>
+      </c>
+      <c r="AE124">
+        <v>10.2917635</v>
+      </c>
+      <c r="AF124">
+        <v>13.9127098</v>
+      </c>
+      <c r="AG124">
+        <v>17.5774844</v>
+      </c>
+      <c r="AH124">
+        <v>21.227876</v>
+      </c>
+      <c r="AI124">
+        <v>13.6594523</v>
+      </c>
+      <c r="AJ124">
+        <v>17.1309745</v>
+      </c>
+      <c r="AK124">
+        <v>13.9115842</v>
+      </c>
+      <c r="AL124">
+        <v>12.8987259</v>
+      </c>
+      <c r="AM124">
+        <v>15.2994503</v>
+      </c>
+      <c r="AN124">
+        <v>14.2817472</v>
+      </c>
+      <c r="AO124">
+        <v>13.9328542</v>
+      </c>
+      <c r="AP124">
+        <v>11.2304792</v>
+      </c>
+      <c r="AQ124">
+        <v>12.1814004</v>
+      </c>
+      <c r="AR124">
+        <v>12.2159577</v>
+      </c>
+      <c r="AS124">
+        <v>15.0243272</v>
+      </c>
+      <c r="AT124">
+        <v>14.3803623</v>
+      </c>
+      <c r="AU124">
+        <v>21.0610408</v>
+      </c>
+      <c r="AV124">
+        <v>13.6898051</v>
+      </c>
+      <c r="AW124">
+        <v>14.4886775</v>
+      </c>
+      <c r="AX124">
+        <v>16.6109142</v>
+      </c>
+      <c r="AY124">
+        <v>15.4748305</v>
+      </c>
+      <c r="BA124">
+        <v>9.5398067</v>
+      </c>
+      <c r="BB124">
+        <v>13.406725</v>
+      </c>
+      <c r="BC124">
+        <v>14.4690956</v>
+      </c>
+      <c r="BD124">
+        <v>13.7298209</v>
+      </c>
+      <c r="BE124">
+        <v>14.4995233</v>
+      </c>
+    </row>
+    <row r="125" spans="1:57">
+      <c r="A125" t="s">
+        <v>179</v>
+      </c>
+      <c r="B125">
+        <v>11.814693</v>
+      </c>
+      <c r="C125">
+        <v>18.7363156</v>
+      </c>
+      <c r="D125">
+        <v>17.670227</v>
+      </c>
+      <c r="F125">
+        <v>15.0548898</v>
+      </c>
+      <c r="G125">
+        <v>11.3314312</v>
+      </c>
+      <c r="H125">
+        <v>15.0712037</v>
+      </c>
+      <c r="I125">
+        <v>15.5639858</v>
+      </c>
+      <c r="J125">
+        <v>16.6083916</v>
+      </c>
+      <c r="K125">
+        <v>14.6426827</v>
+      </c>
+      <c r="L125">
+        <v>11.8639727</v>
+      </c>
+      <c r="M125">
+        <v>16.2637838</v>
+      </c>
+      <c r="O125">
+        <v>9.25</v>
+      </c>
+      <c r="P125">
+        <v>20.4053137</v>
+      </c>
+      <c r="Q125">
+        <v>13.3934708</v>
+      </c>
+      <c r="R125">
+        <v>15.8668252</v>
+      </c>
+      <c r="S125">
+        <v>18.6378651</v>
+      </c>
+      <c r="T125">
+        <v>14.8348661</v>
+      </c>
+      <c r="U125">
+        <v>14.7523711</v>
+      </c>
+      <c r="V125">
+        <v>19.5370663</v>
+      </c>
+      <c r="W125">
+        <v>16.0712625</v>
+      </c>
+      <c r="X125">
+        <v>16.2463057</v>
+      </c>
+      <c r="Y125">
+        <v>10.1835853</v>
+      </c>
+      <c r="Z125">
+        <v>14.0627452</v>
+      </c>
+      <c r="AA125">
+        <v>17.2956312</v>
+      </c>
+      <c r="AB125">
+        <v>14.8490425</v>
+      </c>
+      <c r="AD125">
+        <v>20.4356436</v>
+      </c>
+      <c r="AE125">
+        <v>9.4163891</v>
+      </c>
+      <c r="AF125">
+        <v>14.1992598</v>
+      </c>
+      <c r="AG125">
+        <v>18.5768029</v>
+      </c>
+      <c r="AH125">
+        <v>20.4326523</v>
+      </c>
+      <c r="AI125">
+        <v>13.4968638</v>
+      </c>
+      <c r="AJ125">
+        <v>16.9499312</v>
+      </c>
+      <c r="AK125">
+        <v>13.5927795</v>
+      </c>
+      <c r="AL125">
+        <v>12.5812421</v>
+      </c>
+      <c r="AM125">
+        <v>15.1868031</v>
+      </c>
+      <c r="AN125">
+        <v>14.0842797</v>
+      </c>
+      <c r="AO125">
+        <v>14.1265401</v>
+      </c>
+      <c r="AP125">
+        <v>11.4928076</v>
+      </c>
+      <c r="AQ125">
+        <v>12.0117758</v>
+      </c>
+      <c r="AR125">
+        <v>12.7329193</v>
+      </c>
+      <c r="AS125">
+        <v>14.347615</v>
+      </c>
+      <c r="AT125">
+        <v>14.3411821</v>
+      </c>
+      <c r="AU125">
+        <v>20.3420182</v>
+      </c>
+      <c r="AV125">
+        <v>13.784677</v>
+      </c>
+      <c r="AW125">
+        <v>14.5458575</v>
+      </c>
+      <c r="AX125">
+        <v>17.1316031</v>
+      </c>
+      <c r="AY125">
+        <v>15.1200427</v>
+      </c>
+      <c r="BA125">
+        <v>9.0402217</v>
+      </c>
+      <c r="BB125">
+        <v>13.4631368</v>
+      </c>
+      <c r="BC125">
+        <v>14.2372689</v>
+      </c>
+      <c r="BD125">
+        <v>13.7652473</v>
+      </c>
+      <c r="BE125">
+        <v>14.390123</v>
+      </c>
+    </row>
+    <row r="126" spans="1:57">
+      <c r="A126" t="s">
+        <v>180</v>
+      </c>
+      <c r="B126">
+        <v>11.3832853</v>
+      </c>
+      <c r="C126">
+        <v>19.5490362</v>
+      </c>
+      <c r="D126">
+        <v>17.8246431</v>
+      </c>
+      <c r="F126">
+        <v>15.1424916</v>
+      </c>
+      <c r="G126">
+        <v>11.3773956</v>
+      </c>
+      <c r="H126">
+        <v>14.6181609</v>
+      </c>
+      <c r="I126">
+        <v>15.3120165</v>
+      </c>
+      <c r="J126">
+        <v>15.1728553</v>
+      </c>
+      <c r="K126">
+        <v>15.043592</v>
+      </c>
+      <c r="L126">
+        <v>11.6157393</v>
+      </c>
+      <c r="M126">
+        <v>15.8155882</v>
+      </c>
+      <c r="O126">
+        <v>8.7894249</v>
+      </c>
+      <c r="P126">
+        <v>20.1245942</v>
+      </c>
+      <c r="Q126">
+        <v>13.8141082</v>
+      </c>
+      <c r="R126">
+        <v>15.5056831</v>
+      </c>
+      <c r="S126">
+        <v>18.5247995</v>
+      </c>
+      <c r="T126">
+        <v>14.0363711</v>
+      </c>
+      <c r="U126">
+        <v>15.4925417</v>
+      </c>
+      <c r="V126">
+        <v>19.2268127</v>
+      </c>
+      <c r="W126">
+        <v>16.1316809</v>
+      </c>
+      <c r="X126">
+        <v>15.9695245</v>
+      </c>
+      <c r="Y126">
+        <v>10.2288174</v>
+      </c>
+      <c r="Z126">
+        <v>13.7075491</v>
+      </c>
+      <c r="AA126">
+        <v>17.2119012</v>
+      </c>
+      <c r="AB126">
+        <v>14.9067591</v>
+      </c>
+      <c r="AD126">
+        <v>20.2638172</v>
+      </c>
+      <c r="AE126">
+        <v>9.6901589</v>
+      </c>
+      <c r="AF126">
+        <v>14.3056784</v>
+      </c>
+      <c r="AG126">
+        <v>18.1919969</v>
+      </c>
+      <c r="AH126">
+        <v>19.7387855</v>
+      </c>
+      <c r="AI126">
+        <v>13.6083181</v>
+      </c>
+      <c r="AJ126">
+        <v>16.3335512</v>
+      </c>
+      <c r="AK126">
+        <v>13.917699</v>
+      </c>
+      <c r="AL126">
+        <v>12.9687109</v>
+      </c>
+      <c r="AM126">
+        <v>14.7900317</v>
+      </c>
+      <c r="AN126">
+        <v>14.0925129</v>
+      </c>
+      <c r="AO126">
+        <v>14.2541212</v>
+      </c>
+      <c r="AP126">
+        <v>11.5370577</v>
+      </c>
+      <c r="AQ126">
+        <v>12.0422027</v>
+      </c>
+      <c r="AR126">
+        <v>12.7587101</v>
+      </c>
+      <c r="AS126">
+        <v>14.1460022</v>
+      </c>
+      <c r="AT126">
+        <v>14.4097329</v>
+      </c>
+      <c r="AU126">
+        <v>20.6840599</v>
+      </c>
+      <c r="AV126">
+        <v>13.6182758</v>
+      </c>
+      <c r="AW126">
+        <v>14.6861059</v>
+      </c>
+      <c r="AX126">
+        <v>17.4774932</v>
+      </c>
+      <c r="AY126">
+        <v>14.901903</v>
+      </c>
+      <c r="BA126">
+        <v>9.615384600000001</v>
+      </c>
+      <c r="BB126">
+        <v>13.2416785</v>
+      </c>
+      <c r="BC126">
+        <v>14.2862764</v>
+      </c>
+      <c r="BD126">
+        <v>12.8883871</v>
+      </c>
+      <c r="BE126">
+        <v>15.2005792</v>
+      </c>
+    </row>
+    <row r="127" spans="1:57">
+      <c r="A127" t="s">
+        <v>181</v>
+      </c>
+      <c r="B127">
+        <v>12.0035566</v>
+      </c>
+      <c r="C127">
+        <v>19.7044027</v>
+      </c>
+      <c r="D127">
+        <v>17.9351663</v>
+      </c>
+      <c r="F127">
+        <v>15.6301729</v>
+      </c>
+      <c r="G127">
+        <v>11.3313224</v>
+      </c>
+      <c r="H127">
+        <v>14.6786272</v>
+      </c>
+      <c r="I127">
+        <v>14.8741777</v>
+      </c>
+      <c r="J127">
+        <v>16.1782662</v>
+      </c>
+      <c r="K127">
+        <v>14.8640506</v>
+      </c>
+      <c r="L127">
+        <v>11.5611115</v>
+      </c>
+      <c r="M127">
+        <v>16.0075127</v>
+      </c>
+      <c r="O127">
+        <v>8.7438424</v>
+      </c>
+      <c r="P127">
+        <v>20.119043</v>
+      </c>
+      <c r="Q127">
+        <v>14.0976034</v>
+      </c>
+      <c r="R127">
+        <v>15.0949068</v>
+      </c>
+      <c r="S127">
+        <v>18.27988</v>
+      </c>
+      <c r="T127">
+        <v>14.365135</v>
+      </c>
+      <c r="U127">
+        <v>15.3878522</v>
+      </c>
+      <c r="V127">
+        <v>19.2828626</v>
+      </c>
+      <c r="W127">
+        <v>15.943804</v>
+      </c>
+      <c r="X127">
+        <v>15.8810978</v>
+      </c>
+      <c r="Y127">
+        <v>10.5403525</v>
+      </c>
+      <c r="Z127">
+        <v>13.5969602</v>
+      </c>
+      <c r="AA127">
+        <v>16.3080427</v>
+      </c>
+      <c r="AB127">
+        <v>14.8463573</v>
+      </c>
+      <c r="AD127">
+        <v>19.9377031</v>
+      </c>
+      <c r="AE127">
+        <v>9.8438313</v>
+      </c>
+      <c r="AF127">
+        <v>14.4325211</v>
+      </c>
+      <c r="AG127">
+        <v>18.0181321</v>
+      </c>
+      <c r="AH127">
+        <v>20.3556036</v>
+      </c>
+      <c r="AI127">
+        <v>12.6539624</v>
+      </c>
+      <c r="AJ127">
+        <v>15.9347273</v>
+      </c>
+      <c r="AK127">
+        <v>14.0268622</v>
+      </c>
+      <c r="AL127">
+        <v>12.7631282</v>
+      </c>
+      <c r="AM127">
+        <v>14.4957168</v>
+      </c>
+      <c r="AN127">
+        <v>13.72005</v>
+      </c>
+      <c r="AO127">
+        <v>14.4480335</v>
+      </c>
+      <c r="AP127">
+        <v>11.4184249</v>
+      </c>
+      <c r="AQ127">
+        <v>11.8629735</v>
+      </c>
+      <c r="AR127">
+        <v>10.3846154</v>
+      </c>
+      <c r="AS127">
+        <v>13.4677713</v>
+      </c>
+      <c r="AT127">
+        <v>14.319057</v>
+      </c>
+      <c r="AU127">
+        <v>19.252603</v>
+      </c>
+      <c r="AV127">
+        <v>13.4383922</v>
+      </c>
+      <c r="AW127">
+        <v>14.5067304</v>
+      </c>
+      <c r="AX127">
+        <v>17.6116455</v>
+      </c>
+      <c r="AY127">
+        <v>14.922335</v>
+      </c>
+      <c r="BA127">
+        <v>8.993971999999999</v>
+      </c>
+      <c r="BB127">
+        <v>12.9343328</v>
+      </c>
+      <c r="BC127">
+        <v>13.9741451</v>
+      </c>
+      <c r="BD127">
+        <v>13.6967255</v>
+      </c>
+      <c r="BE127">
+        <v>15.7766241</v>
+      </c>
+    </row>
+    <row r="128" spans="1:57">
+      <c r="A128" t="s">
+        <v>182</v>
+      </c>
+      <c r="B128">
+        <v>13.0201765</v>
+      </c>
+      <c r="C128">
+        <v>19.3907246</v>
+      </c>
+      <c r="D128">
+        <v>18.3076257</v>
+      </c>
+      <c r="F128">
+        <v>15.7920972</v>
+      </c>
+      <c r="G128">
+        <v>11.4733163</v>
+      </c>
+      <c r="H128">
+        <v>14.5098615</v>
+      </c>
+      <c r="I128">
+        <v>14.4362663</v>
+      </c>
+      <c r="J128">
+        <v>16.2077597</v>
+      </c>
+      <c r="K128">
+        <v>14.7579948</v>
+      </c>
+      <c r="L128">
+        <v>11.774065</v>
+      </c>
+      <c r="M128">
+        <v>15.7653073</v>
+      </c>
+      <c r="O128">
+        <v>7.485349</v>
+      </c>
+      <c r="P128">
+        <v>20.3072495</v>
+      </c>
+      <c r="Q128">
+        <v>13.5186865</v>
+      </c>
+      <c r="R128">
+        <v>15.1311186</v>
+      </c>
+      <c r="S128">
+        <v>18.606122</v>
+      </c>
+      <c r="T128">
+        <v>14.5635459</v>
+      </c>
+      <c r="U128">
+        <v>15.2259707</v>
+      </c>
+      <c r="V128">
+        <v>19.2080921</v>
+      </c>
+      <c r="W128">
+        <v>16.1783622</v>
+      </c>
+      <c r="X128">
+        <v>15.674513</v>
+      </c>
+      <c r="Y128">
+        <v>10.5034265</v>
+      </c>
+      <c r="Z128">
+        <v>13.4264022</v>
+      </c>
+      <c r="AA128">
+        <v>16.7609852</v>
+      </c>
+      <c r="AB128">
+        <v>14.9009109</v>
+      </c>
+      <c r="AD128">
+        <v>20.8144855</v>
+      </c>
+      <c r="AE128">
+        <v>10.4296009</v>
+      </c>
+      <c r="AF128">
+        <v>14.3535007</v>
+      </c>
+      <c r="AG128">
+        <v>19.6169035</v>
+      </c>
+      <c r="AH128">
+        <v>20.3654683</v>
+      </c>
+      <c r="AI128">
+        <v>13.0580958</v>
+      </c>
+      <c r="AJ128">
+        <v>15.4762853</v>
+      </c>
+      <c r="AK128">
+        <v>13.2180148</v>
+      </c>
+      <c r="AL128">
+        <v>12.9405504</v>
+      </c>
+      <c r="AM128">
+        <v>14.5441568</v>
+      </c>
+      <c r="AN128">
+        <v>13.5761371</v>
+      </c>
+      <c r="AO128">
+        <v>13.8899385</v>
+      </c>
+      <c r="AP128">
+        <v>11.1351554</v>
+      </c>
+      <c r="AQ128">
+        <v>11.7157836</v>
+      </c>
+      <c r="AS128">
+        <v>13.9287102</v>
+      </c>
+      <c r="AT128">
+        <v>14.4988624</v>
+      </c>
+      <c r="AU128">
+        <v>19.9558536</v>
+      </c>
+      <c r="AV128">
+        <v>13.7041421</v>
+      </c>
+      <c r="AW128">
+        <v>14.4571091</v>
+      </c>
+      <c r="AX128">
+        <v>17.8783984</v>
+      </c>
+      <c r="AY128">
+        <v>14.3251903</v>
+      </c>
+      <c r="BA128">
+        <v>9.468006900000001</v>
+      </c>
+      <c r="BB128">
+        <v>12.8820076</v>
+      </c>
+      <c r="BC128">
+        <v>13.976316</v>
+      </c>
+      <c r="BD128">
+        <v>13.5962756</v>
+      </c>
+      <c r="BE128">
+        <v>15.8181815</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1">
+      <c r="A129" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1">
+      <c r="A130" t="s">
+        <v>184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data up to 11th
</commit_message>
<xml_diff>
--- a/fb-survey-communityState.xlsx
+++ b/fb-survey-communityState.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="188">
   <si>
     <t>Alaska</t>
   </si>
@@ -569,6 +569,15 @@
   </si>
   <si>
     <t>08 06 2020</t>
+  </si>
+  <si>
+    <t>09 06 2020</t>
+  </si>
+  <si>
+    <t>10 06 2020</t>
+  </si>
+  <si>
+    <t>11 06 2020</t>
   </si>
 </sst>
 </file>
@@ -900,7 +909,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BE130"/>
+  <dimension ref="A1:BE133"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -9584,7 +9593,7 @@
         <v>15.0949068</v>
       </c>
       <c r="S127">
-        <v>18.27988</v>
+        <v>18.2865828</v>
       </c>
       <c r="T127">
         <v>14.365135</v>
@@ -9641,7 +9650,7 @@
         <v>12.7631282</v>
       </c>
       <c r="AM127">
-        <v>14.4957168</v>
+        <v>14.4951626</v>
       </c>
       <c r="AN127">
         <v>13.72005</v>
@@ -9709,13 +9718,13 @@
         <v>18.3076257</v>
       </c>
       <c r="F128">
-        <v>15.7920972</v>
+        <v>15.7906661</v>
       </c>
       <c r="G128">
-        <v>11.4733163</v>
+        <v>11.47303</v>
       </c>
       <c r="H128">
-        <v>14.5098615</v>
+        <v>14.5069889</v>
       </c>
       <c r="I128">
         <v>14.4362663</v>
@@ -9727,7 +9736,7 @@
         <v>14.7579948</v>
       </c>
       <c r="L128">
-        <v>11.774065</v>
+        <v>11.7736866</v>
       </c>
       <c r="M128">
         <v>15.7653073</v>
@@ -9742,10 +9751,10 @@
         <v>13.5186865</v>
       </c>
       <c r="R128">
-        <v>15.1311186</v>
+        <v>15.130351</v>
       </c>
       <c r="S128">
-        <v>18.606122</v>
+        <v>18.6131636</v>
       </c>
       <c r="T128">
         <v>14.5635459</v>
@@ -9793,7 +9802,7 @@
         <v>13.0580958</v>
       </c>
       <c r="AJ128">
-        <v>15.4762853</v>
+        <v>15.475009</v>
       </c>
       <c r="AK128">
         <v>13.2180148</v>
@@ -9802,7 +9811,7 @@
         <v>12.9405504</v>
       </c>
       <c r="AM128">
-        <v>14.5441568</v>
+        <v>14.5435281</v>
       </c>
       <c r="AN128">
         <v>13.5761371</v>
@@ -9814,13 +9823,16 @@
         <v>11.1351554</v>
       </c>
       <c r="AQ128">
-        <v>11.7157836</v>
+        <v>11.7189437</v>
+      </c>
+      <c r="AR128">
+        <v>16.6666667</v>
       </c>
       <c r="AS128">
         <v>13.9287102</v>
       </c>
       <c r="AT128">
-        <v>14.4988624</v>
+        <v>14.5069622</v>
       </c>
       <c r="AU128">
         <v>19.9558536</v>
@@ -9832,7 +9844,7 @@
         <v>14.4571091</v>
       </c>
       <c r="AX128">
-        <v>17.8783984</v>
+        <v>17.8924122</v>
       </c>
       <c r="AY128">
         <v>14.3251903</v>
@@ -9853,14 +9865,488 @@
         <v>15.8181815</v>
       </c>
     </row>
-    <row r="129" spans="1:1">
+    <row r="129" spans="1:57">
       <c r="A129" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="130" spans="1:1">
+      <c r="B129">
+        <v>13.3966891</v>
+      </c>
+      <c r="C129">
+        <v>19.551786</v>
+      </c>
+      <c r="D129">
+        <v>17.8413619</v>
+      </c>
+      <c r="F129">
+        <v>16.2745311</v>
+      </c>
+      <c r="G129">
+        <v>11.3958285</v>
+      </c>
+      <c r="H129">
+        <v>14.0148556</v>
+      </c>
+      <c r="I129">
+        <v>14.5096508</v>
+      </c>
+      <c r="J129">
+        <v>16.1547912</v>
+      </c>
+      <c r="K129">
+        <v>14.645359</v>
+      </c>
+      <c r="L129">
+        <v>11.7526909</v>
+      </c>
+      <c r="M129">
+        <v>15.6578749</v>
+      </c>
+      <c r="O129">
+        <v>7.8093812</v>
+      </c>
+      <c r="P129">
+        <v>20.2247116</v>
+      </c>
+      <c r="Q129">
+        <v>14.2099706</v>
+      </c>
+      <c r="R129">
+        <v>14.8746526</v>
+      </c>
+      <c r="S129">
+        <v>19.0197771</v>
+      </c>
+      <c r="T129">
+        <v>14.5482429</v>
+      </c>
+      <c r="U129">
+        <v>14.7450354</v>
+      </c>
+      <c r="V129">
+        <v>19.0637298</v>
+      </c>
+      <c r="W129">
+        <v>15.6230926</v>
+      </c>
+      <c r="X129">
+        <v>15.5382182</v>
+      </c>
+      <c r="Y129">
+        <v>10.2209302</v>
+      </c>
+      <c r="Z129">
+        <v>13.3492913</v>
+      </c>
+      <c r="AA129">
+        <v>16.3383757</v>
+      </c>
+      <c r="AB129">
+        <v>14.8020335</v>
+      </c>
+      <c r="AD129">
+        <v>20.4561248</v>
+      </c>
+      <c r="AE129">
+        <v>9.7618005</v>
+      </c>
+      <c r="AF129">
+        <v>14.3768644</v>
+      </c>
+      <c r="AG129">
+        <v>18.7697725</v>
+      </c>
+      <c r="AH129">
+        <v>21.1396537</v>
+      </c>
+      <c r="AI129">
+        <v>12.1983914</v>
+      </c>
+      <c r="AJ129">
+        <v>15.1161879</v>
+      </c>
+      <c r="AK129">
+        <v>13.332979</v>
+      </c>
+      <c r="AL129">
+        <v>13.660548</v>
+      </c>
+      <c r="AM129">
+        <v>14.2235266</v>
+      </c>
+      <c r="AN129">
+        <v>13.6231201</v>
+      </c>
+      <c r="AO129">
+        <v>14.0414219</v>
+      </c>
+      <c r="AP129">
+        <v>11.4422502</v>
+      </c>
+      <c r="AQ129">
+        <v>11.7920549</v>
+      </c>
+      <c r="AS129">
+        <v>13.7175911</v>
+      </c>
+      <c r="AT129">
+        <v>14.4870187</v>
+      </c>
+      <c r="AU129">
+        <v>19.5797247</v>
+      </c>
+      <c r="AV129">
+        <v>13.6817435</v>
+      </c>
+      <c r="AW129">
+        <v>14.6527513</v>
+      </c>
+      <c r="AX129">
+        <v>17.8005621</v>
+      </c>
+      <c r="AY129">
+        <v>14.5569006</v>
+      </c>
+      <c r="BA129">
+        <v>8.9254684</v>
+      </c>
+      <c r="BB129">
+        <v>12.6542692</v>
+      </c>
+      <c r="BC129">
+        <v>13.4698016</v>
+      </c>
+      <c r="BD129">
+        <v>13.9001569</v>
+      </c>
+      <c r="BE129">
+        <v>15.3266506</v>
+      </c>
+    </row>
+    <row r="130" spans="1:57">
       <c r="A130" t="s">
         <v>184</v>
+      </c>
+      <c r="B130">
+        <v>13.9116719</v>
+      </c>
+      <c r="C130">
+        <v>19.3275917</v>
+      </c>
+      <c r="D130">
+        <v>18.2124461</v>
+      </c>
+      <c r="F130">
+        <v>16.4830531</v>
+      </c>
+      <c r="G130">
+        <v>11.348569</v>
+      </c>
+      <c r="H130">
+        <v>14.0403854</v>
+      </c>
+      <c r="I130">
+        <v>14.4266132</v>
+      </c>
+      <c r="J130">
+        <v>16.581306</v>
+      </c>
+      <c r="K130">
+        <v>15.0073024</v>
+      </c>
+      <c r="L130">
+        <v>11.5862401</v>
+      </c>
+      <c r="M130">
+        <v>15.6111176</v>
+      </c>
+      <c r="O130">
+        <v>8.528513200000001</v>
+      </c>
+      <c r="P130">
+        <v>20.2588454</v>
+      </c>
+      <c r="Q130">
+        <v>13.8997025</v>
+      </c>
+      <c r="R130">
+        <v>14.6645239</v>
+      </c>
+      <c r="S130">
+        <v>19.0685443</v>
+      </c>
+      <c r="T130">
+        <v>14.8131428</v>
+      </c>
+      <c r="U130">
+        <v>15.2412698</v>
+      </c>
+      <c r="V130">
+        <v>18.4916255</v>
+      </c>
+      <c r="W130">
+        <v>15.3152684</v>
+      </c>
+      <c r="X130">
+        <v>15.2524546</v>
+      </c>
+      <c r="Y130">
+        <v>10.3298838</v>
+      </c>
+      <c r="Z130">
+        <v>13.1744174</v>
+      </c>
+      <c r="AA130">
+        <v>16.1353727</v>
+      </c>
+      <c r="AB130">
+        <v>14.7477796</v>
+      </c>
+      <c r="AD130">
+        <v>21.1474806</v>
+      </c>
+      <c r="AE130">
+        <v>9.943261100000001</v>
+      </c>
+      <c r="AF130">
+        <v>14.6895306</v>
+      </c>
+      <c r="AG130">
+        <v>17.9764536</v>
+      </c>
+      <c r="AH130">
+        <v>20.9150219</v>
+      </c>
+      <c r="AI130">
+        <v>12.297391</v>
+      </c>
+      <c r="AJ130">
+        <v>15.0489228</v>
+      </c>
+      <c r="AK130">
+        <v>13.6308568</v>
+      </c>
+      <c r="AL130">
+        <v>13.6533383</v>
+      </c>
+      <c r="AM130">
+        <v>13.9227634</v>
+      </c>
+      <c r="AN130">
+        <v>13.7584017</v>
+      </c>
+      <c r="AO130">
+        <v>14.0260367</v>
+      </c>
+      <c r="AP130">
+        <v>11.3501403</v>
+      </c>
+      <c r="AQ130">
+        <v>11.8950669</v>
+      </c>
+      <c r="AS130">
+        <v>13.3378153</v>
+      </c>
+      <c r="AT130">
+        <v>14.5205048</v>
+      </c>
+      <c r="AU130">
+        <v>20.0684195</v>
+      </c>
+      <c r="AV130">
+        <v>13.6226858</v>
+      </c>
+      <c r="AW130">
+        <v>14.9484815</v>
+      </c>
+      <c r="AX130">
+        <v>17.9805388</v>
+      </c>
+      <c r="AY130">
+        <v>14.5202266</v>
+      </c>
+      <c r="BA130">
+        <v>8.3381668</v>
+      </c>
+      <c r="BB130">
+        <v>12.3891171</v>
+      </c>
+      <c r="BC130">
+        <v>13.3228056</v>
+      </c>
+      <c r="BD130">
+        <v>13.0853577</v>
+      </c>
+      <c r="BE130">
+        <v>14.9665782</v>
+      </c>
+    </row>
+    <row r="131" spans="1:57">
+      <c r="A131" t="s">
+        <v>185</v>
+      </c>
+      <c r="B131">
+        <v>14.4913628</v>
+      </c>
+      <c r="C131">
+        <v>19.9402313</v>
+      </c>
+      <c r="D131">
+        <v>18.1086032</v>
+      </c>
+      <c r="F131">
+        <v>16.5476203</v>
+      </c>
+      <c r="G131">
+        <v>11.2962349</v>
+      </c>
+      <c r="H131">
+        <v>13.9327142</v>
+      </c>
+      <c r="I131">
+        <v>14.2798881</v>
+      </c>
+      <c r="J131">
+        <v>15.625</v>
+      </c>
+      <c r="K131">
+        <v>14.2111012</v>
+      </c>
+      <c r="L131">
+        <v>11.7884436</v>
+      </c>
+      <c r="M131">
+        <v>15.4547589</v>
+      </c>
+      <c r="O131">
+        <v>8.5633947</v>
+      </c>
+      <c r="P131">
+        <v>20.313587</v>
+      </c>
+      <c r="Q131">
+        <v>14.3406705</v>
+      </c>
+      <c r="R131">
+        <v>14.4654193</v>
+      </c>
+      <c r="S131">
+        <v>18.8825783</v>
+      </c>
+      <c r="T131">
+        <v>14.5313118</v>
+      </c>
+      <c r="U131">
+        <v>15.0245709</v>
+      </c>
+      <c r="V131">
+        <v>18.2493735</v>
+      </c>
+      <c r="W131">
+        <v>15.0174044</v>
+      </c>
+      <c r="X131">
+        <v>15.3453029</v>
+      </c>
+      <c r="Y131">
+        <v>10.1209982</v>
+      </c>
+      <c r="Z131">
+        <v>13.1206828</v>
+      </c>
+      <c r="AA131">
+        <v>15.8758346</v>
+      </c>
+      <c r="AB131">
+        <v>14.3983524</v>
+      </c>
+      <c r="AD131">
+        <v>21.2176896</v>
+      </c>
+      <c r="AE131">
+        <v>10.4555128</v>
+      </c>
+      <c r="AF131">
+        <v>14.7950494</v>
+      </c>
+      <c r="AG131">
+        <v>18.3252985</v>
+      </c>
+      <c r="AH131">
+        <v>21.1554369</v>
+      </c>
+      <c r="AI131">
+        <v>12.0874698</v>
+      </c>
+      <c r="AJ131">
+        <v>14.6992655</v>
+      </c>
+      <c r="AK131">
+        <v>14.220647</v>
+      </c>
+      <c r="AL131">
+        <v>13.2396025</v>
+      </c>
+      <c r="AM131">
+        <v>13.3784943</v>
+      </c>
+      <c r="AN131">
+        <v>13.598012</v>
+      </c>
+      <c r="AO131">
+        <v>13.9496459</v>
+      </c>
+      <c r="AP131">
+        <v>11.6229082</v>
+      </c>
+      <c r="AQ131">
+        <v>11.6127365</v>
+      </c>
+      <c r="AS131">
+        <v>13.5426632</v>
+      </c>
+      <c r="AT131">
+        <v>15.0218712</v>
+      </c>
+      <c r="AU131">
+        <v>19.7156971</v>
+      </c>
+      <c r="AV131">
+        <v>13.9147307</v>
+      </c>
+      <c r="AW131">
+        <v>15.1095526</v>
+      </c>
+      <c r="AX131">
+        <v>17.9030771</v>
+      </c>
+      <c r="AY131">
+        <v>14.2341501</v>
+      </c>
+      <c r="BA131">
+        <v>8.667074599999999</v>
+      </c>
+      <c r="BB131">
+        <v>12.4524758</v>
+      </c>
+      <c r="BC131">
+        <v>13.5970998</v>
+      </c>
+      <c r="BD131">
+        <v>13.9478458</v>
+      </c>
+      <c r="BE131">
+        <v>15.1991216</v>
+      </c>
+    </row>
+    <row r="132" spans="1:57">
+      <c r="A132" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="133" spans="1:57">
+      <c r="A133" t="s">
+        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data up to 16th
</commit_message>
<xml_diff>
--- a/fb-survey-communityState.xlsx
+++ b/fb-survey-communityState.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="193">
   <si>
     <t>Alaska</t>
   </si>
@@ -578,6 +578,21 @@
   </si>
   <si>
     <t>11 06 2020</t>
+  </si>
+  <si>
+    <t>12 06 2020</t>
+  </si>
+  <si>
+    <t>13 06 2020</t>
+  </si>
+  <si>
+    <t>14 06 2020</t>
+  </si>
+  <si>
+    <t>15 06 2020</t>
+  </si>
+  <si>
+    <t>16 06 2020</t>
   </si>
 </sst>
 </file>
@@ -909,7 +924,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BE133"/>
+  <dimension ref="A1:BE138"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -9936,7 +9951,7 @@
         <v>10.2209302</v>
       </c>
       <c r="Z129">
-        <v>13.3492913</v>
+        <v>13.3529615</v>
       </c>
       <c r="AA129">
         <v>16.3383757</v>
@@ -9985,6 +10000,9 @@
       </c>
       <c r="AQ129">
         <v>11.7920549</v>
+      </c>
+      <c r="AR129">
+        <v>7.5893467</v>
       </c>
       <c r="AS129">
         <v>13.7175911</v>
@@ -10094,7 +10112,7 @@
         <v>10.3298838</v>
       </c>
       <c r="Z130">
-        <v>13.1744174</v>
+        <v>13.1781499</v>
       </c>
       <c r="AA130">
         <v>16.1353727</v>
@@ -10144,6 +10162,9 @@
       <c r="AQ130">
         <v>11.8950669</v>
       </c>
+      <c r="AR130">
+        <v>10.2485045</v>
+      </c>
       <c r="AS130">
         <v>13.3378153</v>
       </c>
@@ -10178,7 +10199,7 @@
         <v>13.0853577</v>
       </c>
       <c r="BE130">
-        <v>14.9665782</v>
+        <v>14.9564713</v>
       </c>
     </row>
     <row r="131" spans="1:57">
@@ -10195,10 +10216,10 @@
         <v>18.1086032</v>
       </c>
       <c r="F131">
-        <v>16.5476203</v>
+        <v>16.5461133</v>
       </c>
       <c r="G131">
-        <v>11.2962349</v>
+        <v>11.2959453</v>
       </c>
       <c r="H131">
         <v>13.9327142</v>
@@ -10213,13 +10234,13 @@
         <v>14.2111012</v>
       </c>
       <c r="L131">
-        <v>11.7884436</v>
+        <v>11.7876606</v>
       </c>
       <c r="M131">
         <v>15.4547589</v>
       </c>
       <c r="O131">
-        <v>8.5633947</v>
+        <v>8.5590189</v>
       </c>
       <c r="P131">
         <v>20.313587</v>
@@ -10231,7 +10252,7 @@
         <v>14.4654193</v>
       </c>
       <c r="S131">
-        <v>18.8825783</v>
+        <v>18.8809763</v>
       </c>
       <c r="T131">
         <v>14.5313118</v>
@@ -10252,7 +10273,7 @@
         <v>10.1209982</v>
       </c>
       <c r="Z131">
-        <v>13.1206828</v>
+        <v>13.1246331</v>
       </c>
       <c r="AA131">
         <v>15.8758346</v>
@@ -10306,13 +10327,13 @@
         <v>13.5426632</v>
       </c>
       <c r="AT131">
-        <v>15.0218712</v>
+        <v>15.0204726</v>
       </c>
       <c r="AU131">
         <v>19.7156971</v>
       </c>
       <c r="AV131">
-        <v>13.9147307</v>
+        <v>13.9230571</v>
       </c>
       <c r="AW131">
         <v>15.1095526</v>
@@ -10327,26 +10348,816 @@
         <v>8.667074599999999</v>
       </c>
       <c r="BB131">
-        <v>12.4524758</v>
+        <v>12.4514466</v>
       </c>
       <c r="BC131">
         <v>13.5970998</v>
       </c>
       <c r="BD131">
-        <v>13.9478458</v>
+        <v>13.9446283</v>
       </c>
       <c r="BE131">
-        <v>15.1991216</v>
+        <v>15.1876081</v>
       </c>
     </row>
     <row r="132" spans="1:57">
       <c r="A132" t="s">
         <v>186</v>
       </c>
+      <c r="B132">
+        <v>14.2078255</v>
+      </c>
+      <c r="C132">
+        <v>19.301172</v>
+      </c>
+      <c r="D132">
+        <v>17.8812427</v>
+      </c>
+      <c r="F132">
+        <v>17.1699225</v>
+      </c>
+      <c r="G132">
+        <v>11.3159436</v>
+      </c>
+      <c r="H132">
+        <v>13.7565069</v>
+      </c>
+      <c r="I132">
+        <v>13.6173913</v>
+      </c>
+      <c r="J132">
+        <v>14.8976982</v>
+      </c>
+      <c r="K132">
+        <v>13.5141294</v>
+      </c>
+      <c r="L132">
+        <v>11.529806</v>
+      </c>
+      <c r="M132">
+        <v>15.5494627</v>
+      </c>
+      <c r="O132">
+        <v>7.5867426</v>
+      </c>
+      <c r="P132">
+        <v>20.1670333</v>
+      </c>
+      <c r="Q132">
+        <v>14.7044281</v>
+      </c>
+      <c r="R132">
+        <v>14.3339816</v>
+      </c>
+      <c r="S132">
+        <v>18.7015281</v>
+      </c>
+      <c r="T132">
+        <v>14.3837301</v>
+      </c>
+      <c r="U132">
+        <v>15.345495</v>
+      </c>
+      <c r="V132">
+        <v>18.4882367</v>
+      </c>
+      <c r="W132">
+        <v>14.6836525</v>
+      </c>
+      <c r="X132">
+        <v>14.9465457</v>
+      </c>
+      <c r="Y132">
+        <v>10.0928481</v>
+      </c>
+      <c r="Z132">
+        <v>12.7157998</v>
+      </c>
+      <c r="AA132">
+        <v>15.3844612</v>
+      </c>
+      <c r="AB132">
+        <v>14.1121981</v>
+      </c>
+      <c r="AD132">
+        <v>20.6459457</v>
+      </c>
+      <c r="AE132">
+        <v>10.5509873</v>
+      </c>
+      <c r="AF132">
+        <v>14.7784578</v>
+      </c>
+      <c r="AG132">
+        <v>17.6029318</v>
+      </c>
+      <c r="AH132">
+        <v>20.7043035</v>
+      </c>
+      <c r="AI132">
+        <v>12.0955203</v>
+      </c>
+      <c r="AJ132">
+        <v>14.3063212</v>
+      </c>
+      <c r="AK132">
+        <v>13.9300282</v>
+      </c>
+      <c r="AL132">
+        <v>13.4878516</v>
+      </c>
+      <c r="AM132">
+        <v>13.3802825</v>
+      </c>
+      <c r="AN132">
+        <v>13.567387</v>
+      </c>
+      <c r="AO132">
+        <v>14.2578272</v>
+      </c>
+      <c r="AP132">
+        <v>12.0109486</v>
+      </c>
+      <c r="AQ132">
+        <v>11.7041099</v>
+      </c>
+      <c r="AS132">
+        <v>13.3623027</v>
+      </c>
+      <c r="AT132">
+        <v>15.6660148</v>
+      </c>
+      <c r="AU132">
+        <v>21.0719259</v>
+      </c>
+      <c r="AV132">
+        <v>13.9482109</v>
+      </c>
+      <c r="AW132">
+        <v>15.2458642</v>
+      </c>
+      <c r="AX132">
+        <v>17.770569</v>
+      </c>
+      <c r="AY132">
+        <v>14.3638439</v>
+      </c>
+      <c r="BA132">
+        <v>8.7316102</v>
+      </c>
+      <c r="BB132">
+        <v>12.4410437</v>
+      </c>
+      <c r="BC132">
+        <v>13.3063874</v>
+      </c>
+      <c r="BD132">
+        <v>14.3944167</v>
+      </c>
+      <c r="BE132">
+        <v>14.387196</v>
+      </c>
     </row>
     <row r="133" spans="1:57">
       <c r="A133" t="s">
         <v>187</v>
+      </c>
+      <c r="B133">
+        <v>15.4071661</v>
+      </c>
+      <c r="C133">
+        <v>19.97973</v>
+      </c>
+      <c r="D133">
+        <v>17.5865215</v>
+      </c>
+      <c r="F133">
+        <v>17.4152647</v>
+      </c>
+      <c r="G133">
+        <v>11.2590772</v>
+      </c>
+      <c r="H133">
+        <v>13.3875337</v>
+      </c>
+      <c r="I133">
+        <v>13.2490803</v>
+      </c>
+      <c r="J133">
+        <v>15.3795812</v>
+      </c>
+      <c r="K133">
+        <v>13.3096927</v>
+      </c>
+      <c r="L133">
+        <v>11.589119</v>
+      </c>
+      <c r="M133">
+        <v>15.1490648</v>
+      </c>
+      <c r="O133">
+        <v>7.8556807</v>
+      </c>
+      <c r="P133">
+        <v>20.5131229</v>
+      </c>
+      <c r="Q133">
+        <v>13.8497096</v>
+      </c>
+      <c r="R133">
+        <v>14.0785931</v>
+      </c>
+      <c r="S133">
+        <v>18.79548</v>
+      </c>
+      <c r="T133">
+        <v>14.3156073</v>
+      </c>
+      <c r="U133">
+        <v>15.0097051</v>
+      </c>
+      <c r="V133">
+        <v>18.6318984</v>
+      </c>
+      <c r="W133">
+        <v>14.3606388</v>
+      </c>
+      <c r="X133">
+        <v>14.2663854</v>
+      </c>
+      <c r="Y133">
+        <v>10.0711482</v>
+      </c>
+      <c r="Z133">
+        <v>12.4796205</v>
+      </c>
+      <c r="AA133">
+        <v>15.3820211</v>
+      </c>
+      <c r="AB133">
+        <v>13.6507954</v>
+      </c>
+      <c r="AD133">
+        <v>21.050917</v>
+      </c>
+      <c r="AE133">
+        <v>10.0035525</v>
+      </c>
+      <c r="AF133">
+        <v>14.7180546</v>
+      </c>
+      <c r="AG133">
+        <v>17.5037305</v>
+      </c>
+      <c r="AH133">
+        <v>20.8677006</v>
+      </c>
+      <c r="AI133">
+        <v>11.6119483</v>
+      </c>
+      <c r="AJ133">
+        <v>14.2969908</v>
+      </c>
+      <c r="AK133">
+        <v>13.8412321</v>
+      </c>
+      <c r="AL133">
+        <v>12.6325155</v>
+      </c>
+      <c r="AM133">
+        <v>13.0372738</v>
+      </c>
+      <c r="AN133">
+        <v>13.647672</v>
+      </c>
+      <c r="AO133">
+        <v>14.0221268</v>
+      </c>
+      <c r="AP133">
+        <v>11.6657081</v>
+      </c>
+      <c r="AQ133">
+        <v>11.7214128</v>
+      </c>
+      <c r="AS133">
+        <v>12.9219127</v>
+      </c>
+      <c r="AT133">
+        <v>16.1878248</v>
+      </c>
+      <c r="AU133">
+        <v>20.4633716</v>
+      </c>
+      <c r="AV133">
+        <v>13.9762194</v>
+      </c>
+      <c r="AW133">
+        <v>15.2708939</v>
+      </c>
+      <c r="AX133">
+        <v>18.1371273</v>
+      </c>
+      <c r="AY133">
+        <v>14.0725748</v>
+      </c>
+      <c r="BA133">
+        <v>8.659206599999999</v>
+      </c>
+      <c r="BB133">
+        <v>12.4906953</v>
+      </c>
+      <c r="BC133">
+        <v>13.5647435</v>
+      </c>
+      <c r="BD133">
+        <v>13.6116076</v>
+      </c>
+      <c r="BE133">
+        <v>14.8345475</v>
+      </c>
+    </row>
+    <row r="134" spans="1:57">
+      <c r="A134" t="s">
+        <v>188</v>
+      </c>
+      <c r="B134">
+        <v>15.300727</v>
+      </c>
+      <c r="C134">
+        <v>19.5356138</v>
+      </c>
+      <c r="D134">
+        <v>17.6595259</v>
+      </c>
+      <c r="F134">
+        <v>17.6349544</v>
+      </c>
+      <c r="G134">
+        <v>11.3925637</v>
+      </c>
+      <c r="H134">
+        <v>12.9923334</v>
+      </c>
+      <c r="I134">
+        <v>12.9037963</v>
+      </c>
+      <c r="J134">
+        <v>14.083558</v>
+      </c>
+      <c r="K134">
+        <v>12.7772643</v>
+      </c>
+      <c r="L134">
+        <v>11.7384777</v>
+      </c>
+      <c r="M134">
+        <v>15.0601687</v>
+      </c>
+      <c r="O134">
+        <v>8.299899699999999</v>
+      </c>
+      <c r="P134">
+        <v>20.070983</v>
+      </c>
+      <c r="Q134">
+        <v>14.6148805</v>
+      </c>
+      <c r="R134">
+        <v>13.7458832</v>
+      </c>
+      <c r="S134">
+        <v>18.7859837</v>
+      </c>
+      <c r="T134">
+        <v>14.2674471</v>
+      </c>
+      <c r="U134">
+        <v>14.655373</v>
+      </c>
+      <c r="V134">
+        <v>18.7587594</v>
+      </c>
+      <c r="W134">
+        <v>14.4270854</v>
+      </c>
+      <c r="X134">
+        <v>13.9680509</v>
+      </c>
+      <c r="Y134">
+        <v>9.256577399999999</v>
+      </c>
+      <c r="Z134">
+        <v>12.014159</v>
+      </c>
+      <c r="AA134">
+        <v>15.0357303</v>
+      </c>
+      <c r="AB134">
+        <v>14.2304148</v>
+      </c>
+      <c r="AD134">
+        <v>21.0802879</v>
+      </c>
+      <c r="AE134">
+        <v>9.5368245</v>
+      </c>
+      <c r="AF134">
+        <v>14.629002</v>
+      </c>
+      <c r="AG134">
+        <v>17.1493065</v>
+      </c>
+      <c r="AH134">
+        <v>21.3465108</v>
+      </c>
+      <c r="AI134">
+        <v>11.6519174</v>
+      </c>
+      <c r="AJ134">
+        <v>13.9783621</v>
+      </c>
+      <c r="AK134">
+        <v>14.3683957</v>
+      </c>
+      <c r="AL134">
+        <v>12.9616137</v>
+      </c>
+      <c r="AM134">
+        <v>12.9308176</v>
+      </c>
+      <c r="AN134">
+        <v>13.6416097</v>
+      </c>
+      <c r="AO134">
+        <v>14.8479413</v>
+      </c>
+      <c r="AP134">
+        <v>11.7670466</v>
+      </c>
+      <c r="AQ134">
+        <v>11.6616173</v>
+      </c>
+      <c r="AS134">
+        <v>12.9244698</v>
+      </c>
+      <c r="AT134">
+        <v>16.559976</v>
+      </c>
+      <c r="AU134">
+        <v>20.8628418</v>
+      </c>
+      <c r="AV134">
+        <v>13.9550334</v>
+      </c>
+      <c r="AW134">
+        <v>15.7336092</v>
+      </c>
+      <c r="AX134">
+        <v>18.4351064</v>
+      </c>
+      <c r="AY134">
+        <v>13.8164021</v>
+      </c>
+      <c r="BA134">
+        <v>8.528719000000001</v>
+      </c>
+      <c r="BB134">
+        <v>12.6428402</v>
+      </c>
+      <c r="BC134">
+        <v>13.4217538</v>
+      </c>
+      <c r="BD134">
+        <v>14.248871</v>
+      </c>
+      <c r="BE134">
+        <v>14.6055422</v>
+      </c>
+    </row>
+    <row r="135" spans="1:57">
+      <c r="A135" t="s">
+        <v>189</v>
+      </c>
+      <c r="B135">
+        <v>15.1774398</v>
+      </c>
+      <c r="C135">
+        <v>19.4539491</v>
+      </c>
+      <c r="D135">
+        <v>18.0101713</v>
+      </c>
+      <c r="F135">
+        <v>17.9183935</v>
+      </c>
+      <c r="G135">
+        <v>11.4129938</v>
+      </c>
+      <c r="H135">
+        <v>12.7335787</v>
+      </c>
+      <c r="I135">
+        <v>12.680776</v>
+      </c>
+      <c r="J135">
+        <v>14.5371578</v>
+      </c>
+      <c r="K135">
+        <v>12.8865979</v>
+      </c>
+      <c r="L135">
+        <v>11.7591432</v>
+      </c>
+      <c r="M135">
+        <v>15.3592905</v>
+      </c>
+      <c r="O135">
+        <v>8.100558700000001</v>
+      </c>
+      <c r="P135">
+        <v>20.0351179</v>
+      </c>
+      <c r="Q135">
+        <v>14.4814364</v>
+      </c>
+      <c r="R135">
+        <v>13.4698227</v>
+      </c>
+      <c r="S135">
+        <v>18.6605114</v>
+      </c>
+      <c r="T135">
+        <v>13.7331304</v>
+      </c>
+      <c r="U135">
+        <v>14.426606</v>
+      </c>
+      <c r="V135">
+        <v>18.6317649</v>
+      </c>
+      <c r="W135">
+        <v>13.9226582</v>
+      </c>
+      <c r="X135">
+        <v>13.9851683</v>
+      </c>
+      <c r="Y135">
+        <v>9.076433099999999</v>
+      </c>
+      <c r="Z135">
+        <v>11.7842875</v>
+      </c>
+      <c r="AA135">
+        <v>14.9135091</v>
+      </c>
+      <c r="AB135">
+        <v>14.1342852</v>
+      </c>
+      <c r="AD135">
+        <v>21.0962135</v>
+      </c>
+      <c r="AE135">
+        <v>9.824619999999999</v>
+      </c>
+      <c r="AF135">
+        <v>14.9885001</v>
+      </c>
+      <c r="AG135">
+        <v>16.6291366</v>
+      </c>
+      <c r="AH135">
+        <v>20.5507839</v>
+      </c>
+      <c r="AI135">
+        <v>11.5291262</v>
+      </c>
+      <c r="AJ135">
+        <v>13.7300075</v>
+      </c>
+      <c r="AK135">
+        <v>14.0712605</v>
+      </c>
+      <c r="AL135">
+        <v>13.4167147</v>
+      </c>
+      <c r="AM135">
+        <v>12.7142376</v>
+      </c>
+      <c r="AN135">
+        <v>13.6848956</v>
+      </c>
+      <c r="AO135">
+        <v>14.6589586</v>
+      </c>
+      <c r="AP135">
+        <v>11.9241602</v>
+      </c>
+      <c r="AQ135">
+        <v>11.4898137</v>
+      </c>
+      <c r="AS135">
+        <v>11.9037145</v>
+      </c>
+      <c r="AT135">
+        <v>16.960511</v>
+      </c>
+      <c r="AU135">
+        <v>20.3462191</v>
+      </c>
+      <c r="AV135">
+        <v>14.019408</v>
+      </c>
+      <c r="AW135">
+        <v>15.9887428</v>
+      </c>
+      <c r="AX135">
+        <v>18.4734274</v>
+      </c>
+      <c r="AY135">
+        <v>13.6750689</v>
+      </c>
+      <c r="BA135">
+        <v>8.146070699999999</v>
+      </c>
+      <c r="BB135">
+        <v>12.8200266</v>
+      </c>
+      <c r="BC135">
+        <v>13.3065282</v>
+      </c>
+      <c r="BD135">
+        <v>13.661591</v>
+      </c>
+      <c r="BE135">
+        <v>13.6279081</v>
+      </c>
+    </row>
+    <row r="136" spans="1:57">
+      <c r="A136" t="s">
+        <v>190</v>
+      </c>
+      <c r="B136">
+        <v>14.9645809</v>
+      </c>
+      <c r="C136">
+        <v>19.8181272</v>
+      </c>
+      <c r="D136">
+        <v>18.4630463</v>
+      </c>
+      <c r="F136">
+        <v>18.2413088</v>
+      </c>
+      <c r="G136">
+        <v>11.4578952</v>
+      </c>
+      <c r="H136">
+        <v>12.5188231</v>
+      </c>
+      <c r="I136">
+        <v>12.1695906</v>
+      </c>
+      <c r="J136">
+        <v>14.0977444</v>
+      </c>
+      <c r="K136">
+        <v>12.2875517</v>
+      </c>
+      <c r="L136">
+        <v>11.9147423</v>
+      </c>
+      <c r="M136">
+        <v>15.2651201</v>
+      </c>
+      <c r="O136">
+        <v>8.087130699999999</v>
+      </c>
+      <c r="P136">
+        <v>19.4532801</v>
+      </c>
+      <c r="Q136">
+        <v>14.4506336</v>
+      </c>
+      <c r="R136">
+        <v>13.53054</v>
+      </c>
+      <c r="S136">
+        <v>18.5071082</v>
+      </c>
+      <c r="T136">
+        <v>14.0283952</v>
+      </c>
+      <c r="U136">
+        <v>14.5827185</v>
+      </c>
+      <c r="V136">
+        <v>18.5492201</v>
+      </c>
+      <c r="W136">
+        <v>13.3782549</v>
+      </c>
+      <c r="X136">
+        <v>13.7620279</v>
+      </c>
+      <c r="Y136">
+        <v>9.234173200000001</v>
+      </c>
+      <c r="Z136">
+        <v>11.474599</v>
+      </c>
+      <c r="AA136">
+        <v>14.7731333</v>
+      </c>
+      <c r="AB136">
+        <v>13.9514174</v>
+      </c>
+      <c r="AD136">
+        <v>20.5963494</v>
+      </c>
+      <c r="AE136">
+        <v>9.8346175</v>
+      </c>
+      <c r="AF136">
+        <v>14.7292706</v>
+      </c>
+      <c r="AG136">
+        <v>16.7617261</v>
+      </c>
+      <c r="AH136">
+        <v>20.0518177</v>
+      </c>
+      <c r="AI136">
+        <v>11.0003244</v>
+      </c>
+      <c r="AJ136">
+        <v>13.9168783</v>
+      </c>
+      <c r="AK136">
+        <v>14.4731198</v>
+      </c>
+      <c r="AL136">
+        <v>13.0884216</v>
+      </c>
+      <c r="AM136">
+        <v>12.6239328</v>
+      </c>
+      <c r="AN136">
+        <v>13.6194837</v>
+      </c>
+      <c r="AO136">
+        <v>15.3055437</v>
+      </c>
+      <c r="AP136">
+        <v>12.02674</v>
+      </c>
+      <c r="AQ136">
+        <v>11.3726958</v>
+      </c>
+      <c r="AS136">
+        <v>11.7449412</v>
+      </c>
+      <c r="AT136">
+        <v>17.5838335</v>
+      </c>
+      <c r="AU136">
+        <v>20.8173489</v>
+      </c>
+      <c r="AV136">
+        <v>13.9945432</v>
+      </c>
+      <c r="AW136">
+        <v>16.4032226</v>
+      </c>
+      <c r="AX136">
+        <v>18.6003755</v>
+      </c>
+      <c r="AY136">
+        <v>13.4537752</v>
+      </c>
+      <c r="BA136">
+        <v>8.1673332</v>
+      </c>
+      <c r="BB136">
+        <v>13.2115063</v>
+      </c>
+      <c r="BC136">
+        <v>13.4848592</v>
+      </c>
+      <c r="BD136">
+        <v>13.073168</v>
+      </c>
+      <c r="BE136">
+        <v>13.0956232</v>
+      </c>
+    </row>
+    <row r="137" spans="1:57">
+      <c r="A137" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="138" spans="1:57">
+      <c r="A138" t="s">
+        <v>192</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data up to 22
</commit_message>
<xml_diff>
--- a/fb-survey-communityState.xlsx
+++ b/fb-survey-communityState.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="199">
   <si>
     <t>Alaska</t>
   </si>
@@ -593,6 +593,24 @@
   </si>
   <si>
     <t>16 06 2020</t>
+  </si>
+  <si>
+    <t>17 06 2020</t>
+  </si>
+  <si>
+    <t>18 06 2020</t>
+  </si>
+  <si>
+    <t>19 06 2020</t>
+  </si>
+  <si>
+    <t>20 06 2020</t>
+  </si>
+  <si>
+    <t>21 06 2020</t>
+  </si>
+  <si>
+    <t>22 06 2020</t>
   </si>
 </sst>
 </file>
@@ -924,7 +942,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BE138"/>
+  <dimension ref="A1:BE144"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -10323,6 +10341,9 @@
       <c r="AQ131">
         <v>11.6127365</v>
       </c>
+      <c r="AR131">
+        <v>13.3621726</v>
+      </c>
       <c r="AS131">
         <v>13.5426632</v>
       </c>
@@ -10467,7 +10488,7 @@
         <v>13.4878516</v>
       </c>
       <c r="AM132">
-        <v>13.3802825</v>
+        <v>13.3799812</v>
       </c>
       <c r="AN132">
         <v>13.567387</v>
@@ -10480,6 +10501,9 @@
       </c>
       <c r="AQ132">
         <v>11.7041099</v>
+      </c>
+      <c r="AR132">
+        <v>14.6226415</v>
       </c>
       <c r="AS132">
         <v>13.3623027</v>
@@ -10639,6 +10663,9 @@
       <c r="AQ133">
         <v>11.7214128</v>
       </c>
+      <c r="AR133">
+        <v>11.6381778</v>
+      </c>
       <c r="AS133">
         <v>12.9219127</v>
       </c>
@@ -10854,7 +10881,7 @@
         <v>11.4129938</v>
       </c>
       <c r="H135">
-        <v>12.7335787</v>
+        <v>12.7323076</v>
       </c>
       <c r="I135">
         <v>12.680776</v>
@@ -11000,7 +11027,7 @@
         <v>14.9645809</v>
       </c>
       <c r="C136">
-        <v>19.8181272</v>
+        <v>19.8155376</v>
       </c>
       <c r="D136">
         <v>18.4630463</v>
@@ -11009,10 +11036,10 @@
         <v>18.2413088</v>
       </c>
       <c r="G136">
-        <v>11.4578952</v>
+        <v>11.4576207</v>
       </c>
       <c r="H136">
-        <v>12.5188231</v>
+        <v>12.5175809</v>
       </c>
       <c r="I136">
         <v>12.1695906</v>
@@ -11027,7 +11054,7 @@
         <v>11.9147423</v>
       </c>
       <c r="M136">
-        <v>15.2651201</v>
+        <v>15.2638941</v>
       </c>
       <c r="O136">
         <v>8.087130699999999</v>
@@ -11048,7 +11075,7 @@
         <v>14.0283952</v>
       </c>
       <c r="U136">
-        <v>14.5827185</v>
+        <v>14.5807514</v>
       </c>
       <c r="V136">
         <v>18.5492201</v>
@@ -11108,7 +11135,7 @@
         <v>15.3055437</v>
       </c>
       <c r="AP136">
-        <v>12.02674</v>
+        <v>12.0252072</v>
       </c>
       <c r="AQ136">
         <v>11.3726958</v>
@@ -11154,10 +11181,958 @@
       <c r="A137" t="s">
         <v>191</v>
       </c>
+      <c r="B137">
+        <v>15.6149388</v>
+      </c>
+      <c r="C137">
+        <v>19.5283203</v>
+      </c>
+      <c r="D137">
+        <v>18.442629</v>
+      </c>
+      <c r="F137">
+        <v>18.8023214</v>
+      </c>
+      <c r="G137">
+        <v>11.4473773</v>
+      </c>
+      <c r="H137">
+        <v>12.4193695</v>
+      </c>
+      <c r="I137">
+        <v>11.8438359</v>
+      </c>
+      <c r="J137">
+        <v>14.2045455</v>
+      </c>
+      <c r="K137">
+        <v>12.0906236</v>
+      </c>
+      <c r="L137">
+        <v>12.2196539</v>
+      </c>
+      <c r="M137">
+        <v>15.4590936</v>
+      </c>
+      <c r="O137">
+        <v>7.6448498</v>
+      </c>
+      <c r="P137">
+        <v>18.8169343</v>
+      </c>
+      <c r="Q137">
+        <v>14.2532945</v>
+      </c>
+      <c r="R137">
+        <v>13.5544847</v>
+      </c>
+      <c r="S137">
+        <v>18.2489189</v>
+      </c>
+      <c r="T137">
+        <v>14.0046708</v>
+      </c>
+      <c r="U137">
+        <v>14.3636571</v>
+      </c>
+      <c r="V137">
+        <v>18.6298761</v>
+      </c>
+      <c r="W137">
+        <v>13.1804951</v>
+      </c>
+      <c r="X137">
+        <v>14.0895147</v>
+      </c>
+      <c r="Y137">
+        <v>8.690828399999999</v>
+      </c>
+      <c r="Z137">
+        <v>11.2017161</v>
+      </c>
+      <c r="AA137">
+        <v>14.6757238</v>
+      </c>
+      <c r="AB137">
+        <v>14.3026208</v>
+      </c>
+      <c r="AD137">
+        <v>20.7763476</v>
+      </c>
+      <c r="AE137">
+        <v>10.2391625</v>
+      </c>
+      <c r="AF137">
+        <v>14.8888856</v>
+      </c>
+      <c r="AG137">
+        <v>15.7382285</v>
+      </c>
+      <c r="AH137">
+        <v>20.285459</v>
+      </c>
+      <c r="AI137">
+        <v>11.1610793</v>
+      </c>
+      <c r="AJ137">
+        <v>13.4696817</v>
+      </c>
+      <c r="AK137">
+        <v>14.1425695</v>
+      </c>
+      <c r="AL137">
+        <v>12.9820137</v>
+      </c>
+      <c r="AM137">
+        <v>12.4366508</v>
+      </c>
+      <c r="AN137">
+        <v>13.2853985</v>
+      </c>
+      <c r="AO137">
+        <v>15.7899192</v>
+      </c>
+      <c r="AP137">
+        <v>12.0123571</v>
+      </c>
+      <c r="AQ137">
+        <v>11.3780708</v>
+      </c>
+      <c r="AS137">
+        <v>11.8574575</v>
+      </c>
+      <c r="AT137">
+        <v>17.939465</v>
+      </c>
+      <c r="AU137">
+        <v>20.6017187</v>
+      </c>
+      <c r="AV137">
+        <v>13.75597</v>
+      </c>
+      <c r="AW137">
+        <v>16.7361612</v>
+      </c>
+      <c r="AX137">
+        <v>18.5291131</v>
+      </c>
+      <c r="AY137">
+        <v>13.2754233</v>
+      </c>
+      <c r="BA137">
+        <v>7.4195435</v>
+      </c>
+      <c r="BB137">
+        <v>13.4423746</v>
+      </c>
+      <c r="BC137">
+        <v>13.3799606</v>
+      </c>
+      <c r="BD137">
+        <v>13.2352726</v>
+      </c>
+      <c r="BE137">
+        <v>13.8654836</v>
+      </c>
     </row>
     <row r="138" spans="1:57">
       <c r="A138" t="s">
         <v>192</v>
+      </c>
+      <c r="B138">
+        <v>15.0680493</v>
+      </c>
+      <c r="C138">
+        <v>19.6991256</v>
+      </c>
+      <c r="D138">
+        <v>18.7396905</v>
+      </c>
+      <c r="F138">
+        <v>19.0074847</v>
+      </c>
+      <c r="G138">
+        <v>11.4626189</v>
+      </c>
+      <c r="H138">
+        <v>12.5664047</v>
+      </c>
+      <c r="I138">
+        <v>12.0011983</v>
+      </c>
+      <c r="J138">
+        <v>12.8846154</v>
+      </c>
+      <c r="K138">
+        <v>12.2835005</v>
+      </c>
+      <c r="L138">
+        <v>12.3919952</v>
+      </c>
+      <c r="M138">
+        <v>15.8000529</v>
+      </c>
+      <c r="O138">
+        <v>8.358433700000001</v>
+      </c>
+      <c r="P138">
+        <v>19.0493224</v>
+      </c>
+      <c r="Q138">
+        <v>13.9140686</v>
+      </c>
+      <c r="R138">
+        <v>13.4160883</v>
+      </c>
+      <c r="S138">
+        <v>18.4431473</v>
+      </c>
+      <c r="T138">
+        <v>13.8102217</v>
+      </c>
+      <c r="U138">
+        <v>14.8422778</v>
+      </c>
+      <c r="V138">
+        <v>18.9529513</v>
+      </c>
+      <c r="W138">
+        <v>13.2978148</v>
+      </c>
+      <c r="X138">
+        <v>13.8270077</v>
+      </c>
+      <c r="Y138">
+        <v>9.026920199999999</v>
+      </c>
+      <c r="Z138">
+        <v>11.0033129</v>
+      </c>
+      <c r="AA138">
+        <v>14.7446173</v>
+      </c>
+      <c r="AB138">
+        <v>14.3728993</v>
+      </c>
+      <c r="AD138">
+        <v>21.8431047</v>
+      </c>
+      <c r="AE138">
+        <v>10.3112981</v>
+      </c>
+      <c r="AF138">
+        <v>15.225745</v>
+      </c>
+      <c r="AG138">
+        <v>16.4131367</v>
+      </c>
+      <c r="AH138">
+        <v>20.4613024</v>
+      </c>
+      <c r="AI138">
+        <v>11.4009534</v>
+      </c>
+      <c r="AJ138">
+        <v>13.1389045</v>
+      </c>
+      <c r="AK138">
+        <v>14.1548762</v>
+      </c>
+      <c r="AL138">
+        <v>12.9900376</v>
+      </c>
+      <c r="AM138">
+        <v>12.5457224</v>
+      </c>
+      <c r="AN138">
+        <v>13.3639204</v>
+      </c>
+      <c r="AO138">
+        <v>16.1910891</v>
+      </c>
+      <c r="AP138">
+        <v>12.0042083</v>
+      </c>
+      <c r="AQ138">
+        <v>11.3281086</v>
+      </c>
+      <c r="AS138">
+        <v>11.6375364</v>
+      </c>
+      <c r="AT138">
+        <v>18.4908205</v>
+      </c>
+      <c r="AU138">
+        <v>20.4183064</v>
+      </c>
+      <c r="AV138">
+        <v>13.9301211</v>
+      </c>
+      <c r="AW138">
+        <v>17.2901219</v>
+      </c>
+      <c r="AX138">
+        <v>18.8928171</v>
+      </c>
+      <c r="AY138">
+        <v>13.1343996</v>
+      </c>
+      <c r="BA138">
+        <v>8.112098100000001</v>
+      </c>
+      <c r="BB138">
+        <v>13.5410959</v>
+      </c>
+      <c r="BC138">
+        <v>13.5468238</v>
+      </c>
+      <c r="BD138">
+        <v>12.4645669</v>
+      </c>
+      <c r="BE138">
+        <v>14.346529</v>
+      </c>
+    </row>
+    <row r="139" spans="1:57">
+      <c r="A139" t="s">
+        <v>193</v>
+      </c>
+      <c r="B139">
+        <v>15.6052963</v>
+      </c>
+      <c r="C139">
+        <v>20.3457794</v>
+      </c>
+      <c r="D139">
+        <v>18.9336715</v>
+      </c>
+      <c r="F139">
+        <v>19.5502075</v>
+      </c>
+      <c r="G139">
+        <v>11.6152557</v>
+      </c>
+      <c r="H139">
+        <v>12.5942755</v>
+      </c>
+      <c r="I139">
+        <v>12.0476974</v>
+      </c>
+      <c r="J139">
+        <v>13.6822194</v>
+      </c>
+      <c r="K139">
+        <v>12.1043246</v>
+      </c>
+      <c r="L139">
+        <v>12.9842945</v>
+      </c>
+      <c r="M139">
+        <v>15.9223064</v>
+      </c>
+      <c r="O139">
+        <v>8.7925852</v>
+      </c>
+      <c r="P139">
+        <v>19.1730414</v>
+      </c>
+      <c r="Q139">
+        <v>13.6903944</v>
+      </c>
+      <c r="R139">
+        <v>13.4221344</v>
+      </c>
+      <c r="S139">
+        <v>18.7086104</v>
+      </c>
+      <c r="T139">
+        <v>14.41682</v>
+      </c>
+      <c r="U139">
+        <v>15.1817082</v>
+      </c>
+      <c r="V139">
+        <v>19.1760074</v>
+      </c>
+      <c r="W139">
+        <v>12.9771405</v>
+      </c>
+      <c r="X139">
+        <v>13.5839357</v>
+      </c>
+      <c r="Y139">
+        <v>8.8306354</v>
+      </c>
+      <c r="Z139">
+        <v>10.8661799</v>
+      </c>
+      <c r="AA139">
+        <v>14.9491736</v>
+      </c>
+      <c r="AB139">
+        <v>14.6663431</v>
+      </c>
+      <c r="AD139">
+        <v>22.2423731</v>
+      </c>
+      <c r="AE139">
+        <v>10.7033158</v>
+      </c>
+      <c r="AF139">
+        <v>15.5663568</v>
+      </c>
+      <c r="AG139">
+        <v>16.6079784</v>
+      </c>
+      <c r="AH139">
+        <v>19.7499065</v>
+      </c>
+      <c r="AI139">
+        <v>11.2616311</v>
+      </c>
+      <c r="AJ139">
+        <v>13.1114203</v>
+      </c>
+      <c r="AK139">
+        <v>14.437439</v>
+      </c>
+      <c r="AL139">
+        <v>13.1227802</v>
+      </c>
+      <c r="AM139">
+        <v>12.2138494</v>
+      </c>
+      <c r="AN139">
+        <v>13.4502023</v>
+      </c>
+      <c r="AO139">
+        <v>16.5600298</v>
+      </c>
+      <c r="AP139">
+        <v>11.5623539</v>
+      </c>
+      <c r="AQ139">
+        <v>11.2999319</v>
+      </c>
+      <c r="AS139">
+        <v>11.6725328</v>
+      </c>
+      <c r="AT139">
+        <v>18.6366866</v>
+      </c>
+      <c r="AU139">
+        <v>19.9467344</v>
+      </c>
+      <c r="AV139">
+        <v>14.1671142</v>
+      </c>
+      <c r="AW139">
+        <v>18.3555256</v>
+      </c>
+      <c r="AX139">
+        <v>19.0871463</v>
+      </c>
+      <c r="AY139">
+        <v>13.2600756</v>
+      </c>
+      <c r="BA139">
+        <v>8.133823700000001</v>
+      </c>
+      <c r="BB139">
+        <v>13.400099</v>
+      </c>
+      <c r="BC139">
+        <v>13.918514</v>
+      </c>
+      <c r="BD139">
+        <v>12.9388228</v>
+      </c>
+      <c r="BE139">
+        <v>14.6572575</v>
+      </c>
+    </row>
+    <row r="140" spans="1:57">
+      <c r="A140" t="s">
+        <v>194</v>
+      </c>
+      <c r="B140">
+        <v>15.7637076</v>
+      </c>
+      <c r="C140">
+        <v>20.3321878</v>
+      </c>
+      <c r="D140">
+        <v>19.1347461</v>
+      </c>
+      <c r="F140">
+        <v>19.8888276</v>
+      </c>
+      <c r="G140">
+        <v>12.0209684</v>
+      </c>
+      <c r="H140">
+        <v>12.8524218</v>
+      </c>
+      <c r="I140">
+        <v>12.0209689</v>
+      </c>
+      <c r="J140">
+        <v>13.4013605</v>
+      </c>
+      <c r="K140">
+        <v>12.3030584</v>
+      </c>
+      <c r="L140">
+        <v>13.4168713</v>
+      </c>
+      <c r="M140">
+        <v>16.1857632</v>
+      </c>
+      <c r="O140">
+        <v>8.2910751</v>
+      </c>
+      <c r="P140">
+        <v>18.3994708</v>
+      </c>
+      <c r="Q140">
+        <v>14.0356044</v>
+      </c>
+      <c r="R140">
+        <v>13.499991</v>
+      </c>
+      <c r="S140">
+        <v>18.4196807</v>
+      </c>
+      <c r="T140">
+        <v>14.6683156</v>
+      </c>
+      <c r="U140">
+        <v>15.0604059</v>
+      </c>
+      <c r="V140">
+        <v>19.4530328</v>
+      </c>
+      <c r="W140">
+        <v>12.6542629</v>
+      </c>
+      <c r="X140">
+        <v>13.6196414</v>
+      </c>
+      <c r="Y140">
+        <v>9.153005500000001</v>
+      </c>
+      <c r="Z140">
+        <v>10.8909042</v>
+      </c>
+      <c r="AA140">
+        <v>15.0131008</v>
+      </c>
+      <c r="AB140">
+        <v>14.8439265</v>
+      </c>
+      <c r="AD140">
+        <v>22.1329414</v>
+      </c>
+      <c r="AE140">
+        <v>10.691112</v>
+      </c>
+      <c r="AF140">
+        <v>15.5337024</v>
+      </c>
+      <c r="AG140">
+        <v>15.9935856</v>
+      </c>
+      <c r="AH140">
+        <v>19.5951362</v>
+      </c>
+      <c r="AI140">
+        <v>11.1190818</v>
+      </c>
+      <c r="AJ140">
+        <v>12.837067</v>
+      </c>
+      <c r="AK140">
+        <v>14.9511402</v>
+      </c>
+      <c r="AL140">
+        <v>13.6608688</v>
+      </c>
+      <c r="AM140">
+        <v>12.2546746</v>
+      </c>
+      <c r="AN140">
+        <v>13.0820181</v>
+      </c>
+      <c r="AO140">
+        <v>17.6449543</v>
+      </c>
+      <c r="AP140">
+        <v>11.7066135</v>
+      </c>
+      <c r="AQ140">
+        <v>11.2940544</v>
+      </c>
+      <c r="AS140">
+        <v>11.7879966</v>
+      </c>
+      <c r="AT140">
+        <v>19.3322409</v>
+      </c>
+      <c r="AU140">
+        <v>21.1851886</v>
+      </c>
+      <c r="AV140">
+        <v>14.5164984</v>
+      </c>
+      <c r="AW140">
+        <v>19.2173408</v>
+      </c>
+      <c r="AX140">
+        <v>18.9721588</v>
+      </c>
+      <c r="AY140">
+        <v>13.6086623</v>
+      </c>
+      <c r="BA140">
+        <v>9.355458199999999</v>
+      </c>
+      <c r="BB140">
+        <v>13.3346916</v>
+      </c>
+      <c r="BC140">
+        <v>13.5697173</v>
+      </c>
+      <c r="BD140">
+        <v>13.2590809</v>
+      </c>
+      <c r="BE140">
+        <v>14.8673203</v>
+      </c>
+    </row>
+    <row r="141" spans="1:57">
+      <c r="A141" t="s">
+        <v>195</v>
+      </c>
+      <c r="B141">
+        <v>15.6911142</v>
+      </c>
+      <c r="C141">
+        <v>20.5188878</v>
+      </c>
+      <c r="D141">
+        <v>19.4440121</v>
+      </c>
+      <c r="F141">
+        <v>20.4707148</v>
+      </c>
+      <c r="G141">
+        <v>12.0936925</v>
+      </c>
+      <c r="H141">
+        <v>13.0305609</v>
+      </c>
+      <c r="I141">
+        <v>12.1035387</v>
+      </c>
+      <c r="J141">
+        <v>14.4787645</v>
+      </c>
+      <c r="K141">
+        <v>12.8211462</v>
+      </c>
+      <c r="L141">
+        <v>13.8231764</v>
+      </c>
+      <c r="M141">
+        <v>16.5580787</v>
+      </c>
+      <c r="O141">
+        <v>9.0078329</v>
+      </c>
+      <c r="P141">
+        <v>19.2694904</v>
+      </c>
+      <c r="Q141">
+        <v>14.5680868</v>
+      </c>
+      <c r="R141">
+        <v>13.3354445</v>
+      </c>
+      <c r="S141">
+        <v>18.6318073</v>
+      </c>
+      <c r="T141">
+        <v>15.2372502</v>
+      </c>
+      <c r="U141">
+        <v>15.4480315</v>
+      </c>
+      <c r="V141">
+        <v>19.9544709</v>
+      </c>
+      <c r="W141">
+        <v>12.3700826</v>
+      </c>
+      <c r="X141">
+        <v>13.9466109</v>
+      </c>
+      <c r="Y141">
+        <v>8.791691</v>
+      </c>
+      <c r="Z141">
+        <v>10.6963159</v>
+      </c>
+      <c r="AA141">
+        <v>15.139835</v>
+      </c>
+      <c r="AB141">
+        <v>15.4080429</v>
+      </c>
+      <c r="AD141">
+        <v>22.1583041</v>
+      </c>
+      <c r="AE141">
+        <v>11.9398349</v>
+      </c>
+      <c r="AF141">
+        <v>15.6684567</v>
+      </c>
+      <c r="AG141">
+        <v>16.0921332</v>
+      </c>
+      <c r="AH141">
+        <v>18.9478719</v>
+      </c>
+      <c r="AI141">
+        <v>11.3308801</v>
+      </c>
+      <c r="AJ141">
+        <v>12.8977338</v>
+      </c>
+      <c r="AK141">
+        <v>14.2519614</v>
+      </c>
+      <c r="AL141">
+        <v>13.6566247</v>
+      </c>
+      <c r="AM141">
+        <v>12.1808948</v>
+      </c>
+      <c r="AN141">
+        <v>13.0037343</v>
+      </c>
+      <c r="AO141">
+        <v>18.0259254</v>
+      </c>
+      <c r="AP141">
+        <v>11.7626904</v>
+      </c>
+      <c r="AQ141">
+        <v>11.4475768</v>
+      </c>
+      <c r="AS141">
+        <v>11.8889121</v>
+      </c>
+      <c r="AT141">
+        <v>20.2169335</v>
+      </c>
+      <c r="AU141">
+        <v>21.3479031</v>
+      </c>
+      <c r="AV141">
+        <v>14.6958387</v>
+      </c>
+      <c r="AW141">
+        <v>20.1087938</v>
+      </c>
+      <c r="AX141">
+        <v>19.1362719</v>
+      </c>
+      <c r="AY141">
+        <v>13.4989403</v>
+      </c>
+      <c r="BA141">
+        <v>9.2434162</v>
+      </c>
+      <c r="BB141">
+        <v>13.3152779</v>
+      </c>
+      <c r="BC141">
+        <v>13.7299775</v>
+      </c>
+      <c r="BD141">
+        <v>13.1334905</v>
+      </c>
+      <c r="BE141">
+        <v>14.1792196</v>
+      </c>
+    </row>
+    <row r="142" spans="1:57">
+      <c r="A142" t="s">
+        <v>196</v>
+      </c>
+      <c r="B142">
+        <v>15.6647808</v>
+      </c>
+      <c r="C142">
+        <v>20.760556</v>
+      </c>
+      <c r="D142">
+        <v>20.2102959</v>
+      </c>
+      <c r="F142">
+        <v>21.1602242</v>
+      </c>
+      <c r="G142">
+        <v>12.2418795</v>
+      </c>
+      <c r="H142">
+        <v>13.2127952</v>
+      </c>
+      <c r="I142">
+        <v>11.8537964</v>
+      </c>
+      <c r="J142">
+        <v>13.5994587</v>
+      </c>
+      <c r="K142">
+        <v>13.1284916</v>
+      </c>
+      <c r="L142">
+        <v>14.4759983</v>
+      </c>
+      <c r="M142">
+        <v>16.6395388</v>
+      </c>
+      <c r="O142">
+        <v>8.985429</v>
+      </c>
+      <c r="P142">
+        <v>19.5761948</v>
+      </c>
+      <c r="Q142">
+        <v>14.9041295</v>
+      </c>
+      <c r="R142">
+        <v>13.3006391</v>
+      </c>
+      <c r="S142">
+        <v>18.6298605</v>
+      </c>
+      <c r="T142">
+        <v>15.4976721</v>
+      </c>
+      <c r="U142">
+        <v>15.2144724</v>
+      </c>
+      <c r="V142">
+        <v>19.9447108</v>
+      </c>
+      <c r="W142">
+        <v>12.1804351</v>
+      </c>
+      <c r="X142">
+        <v>13.6294858</v>
+      </c>
+      <c r="Y142">
+        <v>9.172030400000001</v>
+      </c>
+      <c r="Z142">
+        <v>10.7757837</v>
+      </c>
+      <c r="AA142">
+        <v>14.9163279</v>
+      </c>
+      <c r="AB142">
+        <v>15.1062203</v>
+      </c>
+      <c r="AD142">
+        <v>22.8177464</v>
+      </c>
+      <c r="AE142">
+        <v>11.1284749</v>
+      </c>
+      <c r="AF142">
+        <v>16.1250255</v>
+      </c>
+      <c r="AG142">
+        <v>17.2779457</v>
+      </c>
+      <c r="AH142">
+        <v>18.8760784</v>
+      </c>
+      <c r="AI142">
+        <v>11.112898</v>
+      </c>
+      <c r="AJ142">
+        <v>12.6808796</v>
+      </c>
+      <c r="AK142">
+        <v>13.8305469</v>
+      </c>
+      <c r="AL142">
+        <v>13.7830959</v>
+      </c>
+      <c r="AM142">
+        <v>12.1841492</v>
+      </c>
+      <c r="AN142">
+        <v>12.7262508</v>
+      </c>
+      <c r="AO142">
+        <v>19.1477569</v>
+      </c>
+      <c r="AP142">
+        <v>11.8581664</v>
+      </c>
+      <c r="AQ142">
+        <v>11.3918073</v>
+      </c>
+      <c r="AS142">
+        <v>11.8782537</v>
+      </c>
+      <c r="AT142">
+        <v>20.9100572</v>
+      </c>
+      <c r="AU142">
+        <v>20.0406169</v>
+      </c>
+      <c r="AV142">
+        <v>15.0080442</v>
+      </c>
+      <c r="AW142">
+        <v>21.0346173</v>
+      </c>
+      <c r="AX142">
+        <v>18.9995117</v>
+      </c>
+      <c r="AY142">
+        <v>13.6588603</v>
+      </c>
+      <c r="BA142">
+        <v>9.3976778</v>
+      </c>
+      <c r="BB142">
+        <v>13.2376404</v>
+      </c>
+      <c r="BC142">
+        <v>13.7470551</v>
+      </c>
+      <c r="BD142">
+        <v>13.0761004</v>
+      </c>
+      <c r="BE142">
+        <v>14.7427201</v>
+      </c>
+    </row>
+    <row r="143" spans="1:57">
+      <c r="A143" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="144" spans="1:57">
+      <c r="A144" t="s">
+        <v>198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data up to 26
</commit_message>
<xml_diff>
--- a/fb-survey-communityState.xlsx
+++ b/fb-survey-communityState.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="203">
   <si>
     <t>Alaska</t>
   </si>
@@ -611,6 +611,18 @@
   </si>
   <si>
     <t>22 06 2020</t>
+  </si>
+  <si>
+    <t>23 06 2020</t>
+  </si>
+  <si>
+    <t>24 06 2020</t>
+  </si>
+  <si>
+    <t>25 06 2020</t>
+  </si>
+  <si>
+    <t>26 06 2020</t>
   </si>
 </sst>
 </file>
@@ -942,7 +954,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BE144"/>
+  <dimension ref="A1:BE148"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -10824,6 +10836,9 @@
       <c r="AQ134">
         <v>11.6616173</v>
       </c>
+      <c r="AR134">
+        <v>8.8462104</v>
+      </c>
       <c r="AS134">
         <v>12.9244698</v>
       </c>
@@ -10982,6 +10997,9 @@
       <c r="AQ135">
         <v>11.4898137</v>
       </c>
+      <c r="AR135">
+        <v>10.5506085</v>
+      </c>
       <c r="AS135">
         <v>11.9037145</v>
       </c>
@@ -11140,6 +11158,9 @@
       <c r="AQ136">
         <v>11.3726958</v>
       </c>
+      <c r="AR136">
+        <v>14.356492</v>
+      </c>
       <c r="AS136">
         <v>11.7449412</v>
       </c>
@@ -11984,7 +12005,7 @@
         <v>21.1602242</v>
       </c>
       <c r="G142">
-        <v>12.2418795</v>
+        <v>12.2405909</v>
       </c>
       <c r="H142">
         <v>13.2127952</v>
@@ -12129,10 +12150,795 @@
       <c r="A143" t="s">
         <v>197</v>
       </c>
+      <c r="B143">
+        <v>16.4300923</v>
+      </c>
+      <c r="C143">
+        <v>21.1817963</v>
+      </c>
+      <c r="D143">
+        <v>20.2397725</v>
+      </c>
+      <c r="F143">
+        <v>22.149584</v>
+      </c>
+      <c r="G143">
+        <v>12.4251331</v>
+      </c>
+      <c r="H143">
+        <v>13.199867</v>
+      </c>
+      <c r="I143">
+        <v>11.9194381</v>
+      </c>
+      <c r="J143">
+        <v>14.3870968</v>
+      </c>
+      <c r="K143">
+        <v>13.1213255</v>
+      </c>
+      <c r="L143">
+        <v>15.0895932</v>
+      </c>
+      <c r="M143">
+        <v>16.8905516</v>
+      </c>
+      <c r="O143">
+        <v>9.6175166</v>
+      </c>
+      <c r="P143">
+        <v>19.5793223</v>
+      </c>
+      <c r="Q143">
+        <v>15.1881238</v>
+      </c>
+      <c r="R143">
+        <v>13.2566567</v>
+      </c>
+      <c r="S143">
+        <v>18.8726161</v>
+      </c>
+      <c r="T143">
+        <v>15.374564</v>
+      </c>
+      <c r="U143">
+        <v>15.7300681</v>
+      </c>
+      <c r="V143">
+        <v>21.0845323</v>
+      </c>
+      <c r="W143">
+        <v>12.2803712</v>
+      </c>
+      <c r="X143">
+        <v>13.4317781</v>
+      </c>
+      <c r="Y143">
+        <v>9.1019311</v>
+      </c>
+      <c r="Z143">
+        <v>10.6787645</v>
+      </c>
+      <c r="AA143">
+        <v>14.4727302</v>
+      </c>
+      <c r="AB143">
+        <v>15.8673754</v>
+      </c>
+      <c r="AD143">
+        <v>23.3105273</v>
+      </c>
+      <c r="AE143">
+        <v>12.0806163</v>
+      </c>
+      <c r="AF143">
+        <v>16.6446172</v>
+      </c>
+      <c r="AG143">
+        <v>16.7647578</v>
+      </c>
+      <c r="AH143">
+        <v>18.7169639</v>
+      </c>
+      <c r="AI143">
+        <v>10.926004</v>
+      </c>
+      <c r="AJ143">
+        <v>12.7245802</v>
+      </c>
+      <c r="AK143">
+        <v>14.3913285</v>
+      </c>
+      <c r="AL143">
+        <v>13.5518031</v>
+      </c>
+      <c r="AM143">
+        <v>12.2356187</v>
+      </c>
+      <c r="AN143">
+        <v>12.9495034</v>
+      </c>
+      <c r="AO143">
+        <v>19.6064668</v>
+      </c>
+      <c r="AP143">
+        <v>11.2915817</v>
+      </c>
+      <c r="AQ143">
+        <v>11.3086483</v>
+      </c>
+      <c r="AS143">
+        <v>11.5487716</v>
+      </c>
+      <c r="AT143">
+        <v>21.9870886</v>
+      </c>
+      <c r="AU143">
+        <v>19.3609592</v>
+      </c>
+      <c r="AV143">
+        <v>15.189681</v>
+      </c>
+      <c r="AW143">
+        <v>22.1632916</v>
+      </c>
+      <c r="AX143">
+        <v>19.5408345</v>
+      </c>
+      <c r="AY143">
+        <v>13.7730427</v>
+      </c>
+      <c r="BA143">
+        <v>10.388223</v>
+      </c>
+      <c r="BB143">
+        <v>13.1412397</v>
+      </c>
+      <c r="BC143">
+        <v>13.8785426</v>
+      </c>
+      <c r="BD143">
+        <v>13.5789521</v>
+      </c>
+      <c r="BE143">
+        <v>15.5949872</v>
+      </c>
     </row>
     <row r="144" spans="1:57">
       <c r="A144" t="s">
         <v>198</v>
+      </c>
+      <c r="B144">
+        <v>17.0463174</v>
+      </c>
+      <c r="C144">
+        <v>21.1564028</v>
+      </c>
+      <c r="D144">
+        <v>20.2310999</v>
+      </c>
+      <c r="F144">
+        <v>23.0040644</v>
+      </c>
+      <c r="G144">
+        <v>12.775418</v>
+      </c>
+      <c r="H144">
+        <v>12.9222858</v>
+      </c>
+      <c r="I144">
+        <v>11.4963504</v>
+      </c>
+      <c r="J144">
+        <v>13.4214186</v>
+      </c>
+      <c r="K144">
+        <v>13.5416667</v>
+      </c>
+      <c r="L144">
+        <v>15.8324116</v>
+      </c>
+      <c r="M144">
+        <v>17.2471243</v>
+      </c>
+      <c r="O144">
+        <v>9.894304200000001</v>
+      </c>
+      <c r="P144">
+        <v>20.1258308</v>
+      </c>
+      <c r="Q144">
+        <v>16.1170344</v>
+      </c>
+      <c r="R144">
+        <v>13.4225995</v>
+      </c>
+      <c r="S144">
+        <v>18.6094995</v>
+      </c>
+      <c r="T144">
+        <v>16.0758593</v>
+      </c>
+      <c r="U144">
+        <v>15.6757648</v>
+      </c>
+      <c r="V144">
+        <v>21.2745764</v>
+      </c>
+      <c r="W144">
+        <v>11.8854505</v>
+      </c>
+      <c r="X144">
+        <v>13.5907417</v>
+      </c>
+      <c r="Y144">
+        <v>9.627515799999999</v>
+      </c>
+      <c r="Z144">
+        <v>10.7857541</v>
+      </c>
+      <c r="AA144">
+        <v>14.4854168</v>
+      </c>
+      <c r="AB144">
+        <v>15.3933595</v>
+      </c>
+      <c r="AD144">
+        <v>24.0709086</v>
+      </c>
+      <c r="AE144">
+        <v>13.2498915</v>
+      </c>
+      <c r="AF144">
+        <v>16.8520224</v>
+      </c>
+      <c r="AG144">
+        <v>17.1252175</v>
+      </c>
+      <c r="AH144">
+        <v>18.0246439</v>
+      </c>
+      <c r="AI144">
+        <v>10.3153304</v>
+      </c>
+      <c r="AJ144">
+        <v>12.4973671</v>
+      </c>
+      <c r="AK144">
+        <v>14.3150808</v>
+      </c>
+      <c r="AL144">
+        <v>14.3441225</v>
+      </c>
+      <c r="AM144">
+        <v>12.1483419</v>
+      </c>
+      <c r="AN144">
+        <v>13.002053</v>
+      </c>
+      <c r="AO144">
+        <v>19.538884</v>
+      </c>
+      <c r="AP144">
+        <v>11.5369845</v>
+      </c>
+      <c r="AQ144">
+        <v>11.3603624</v>
+      </c>
+      <c r="AS144">
+        <v>10.9600925</v>
+      </c>
+      <c r="AT144">
+        <v>22.9594752</v>
+      </c>
+      <c r="AU144">
+        <v>19.4715984</v>
+      </c>
+      <c r="AV144">
+        <v>15.836489</v>
+      </c>
+      <c r="AW144">
+        <v>22.9719406</v>
+      </c>
+      <c r="AX144">
+        <v>19.9300668</v>
+      </c>
+      <c r="AY144">
+        <v>14.1189323</v>
+      </c>
+      <c r="BA144">
+        <v>10.3096462</v>
+      </c>
+      <c r="BB144">
+        <v>13.474175</v>
+      </c>
+      <c r="BC144">
+        <v>14.1179391</v>
+      </c>
+      <c r="BD144">
+        <v>14.2830295</v>
+      </c>
+      <c r="BE144">
+        <v>15.089086</v>
+      </c>
+    </row>
+    <row r="145" spans="1:57">
+      <c r="A145" t="s">
+        <v>199</v>
+      </c>
+      <c r="B145">
+        <v>17.3165138</v>
+      </c>
+      <c r="C145">
+        <v>22.0360745</v>
+      </c>
+      <c r="D145">
+        <v>20.1803961</v>
+      </c>
+      <c r="F145">
+        <v>24.1166012</v>
+      </c>
+      <c r="G145">
+        <v>13.0016802</v>
+      </c>
+      <c r="H145">
+        <v>13.2370663</v>
+      </c>
+      <c r="I145">
+        <v>11.3911743</v>
+      </c>
+      <c r="J145">
+        <v>15.6716418</v>
+      </c>
+      <c r="K145">
+        <v>13.5115725</v>
+      </c>
+      <c r="L145">
+        <v>16.91313</v>
+      </c>
+      <c r="M145">
+        <v>17.6445627</v>
+      </c>
+      <c r="O145">
+        <v>10.3076923</v>
+      </c>
+      <c r="P145">
+        <v>20.4799191</v>
+      </c>
+      <c r="Q145">
+        <v>16.1706377</v>
+      </c>
+      <c r="R145">
+        <v>13.1358945</v>
+      </c>
+      <c r="S145">
+        <v>18.5500694</v>
+      </c>
+      <c r="T145">
+        <v>15.7639909</v>
+      </c>
+      <c r="U145">
+        <v>15.7251752</v>
+      </c>
+      <c r="V145">
+        <v>22.0776219</v>
+      </c>
+      <c r="W145">
+        <v>11.4029664</v>
+      </c>
+      <c r="X145">
+        <v>13.1204554</v>
+      </c>
+      <c r="Y145">
+        <v>9.6080725</v>
+      </c>
+      <c r="Z145">
+        <v>10.848253</v>
+      </c>
+      <c r="AA145">
+        <v>15.1191711</v>
+      </c>
+      <c r="AB145">
+        <v>15.5561748</v>
+      </c>
+      <c r="AD145">
+        <v>24.340724</v>
+      </c>
+      <c r="AE145">
+        <v>13.1766286</v>
+      </c>
+      <c r="AF145">
+        <v>16.9959595</v>
+      </c>
+      <c r="AG145">
+        <v>17.3701245</v>
+      </c>
+      <c r="AH145">
+        <v>18.1533888</v>
+      </c>
+      <c r="AI145">
+        <v>10.3858078</v>
+      </c>
+      <c r="AJ145">
+        <v>12.6874065</v>
+      </c>
+      <c r="AK145">
+        <v>15.0644002</v>
+      </c>
+      <c r="AL145">
+        <v>15.2765066</v>
+      </c>
+      <c r="AM145">
+        <v>12.0733555</v>
+      </c>
+      <c r="AN145">
+        <v>12.9759208</v>
+      </c>
+      <c r="AO145">
+        <v>20.3452846</v>
+      </c>
+      <c r="AP145">
+        <v>11.3683295</v>
+      </c>
+      <c r="AQ145">
+        <v>11.5125593</v>
+      </c>
+      <c r="AS145">
+        <v>10.8506175</v>
+      </c>
+      <c r="AT145">
+        <v>23.40987</v>
+      </c>
+      <c r="AU145">
+        <v>20.7864045</v>
+      </c>
+      <c r="AV145">
+        <v>16.032284</v>
+      </c>
+      <c r="AW145">
+        <v>24.1767046</v>
+      </c>
+      <c r="AX145">
+        <v>20.2066568</v>
+      </c>
+      <c r="AY145">
+        <v>14.1157567</v>
+      </c>
+      <c r="BA145">
+        <v>10.2154649</v>
+      </c>
+      <c r="BB145">
+        <v>13.279306</v>
+      </c>
+      <c r="BC145">
+        <v>13.9073914</v>
+      </c>
+      <c r="BD145">
+        <v>13.5028546</v>
+      </c>
+      <c r="BE145">
+        <v>15.2606344</v>
+      </c>
+    </row>
+    <row r="146" spans="1:57">
+      <c r="A146" t="s">
+        <v>200</v>
+      </c>
+      <c r="B146">
+        <v>17.0936749</v>
+      </c>
+      <c r="C146">
+        <v>22.7740105</v>
+      </c>
+      <c r="D146">
+        <v>21.1436974</v>
+      </c>
+      <c r="F146">
+        <v>25.2981312</v>
+      </c>
+      <c r="G146">
+        <v>13.5824354</v>
+      </c>
+      <c r="H146">
+        <v>13.2388967</v>
+      </c>
+      <c r="I146">
+        <v>11.0983632</v>
+      </c>
+      <c r="J146">
+        <v>15.21181</v>
+      </c>
+      <c r="K146">
+        <v>14.2899761</v>
+      </c>
+      <c r="L146">
+        <v>17.7022691</v>
+      </c>
+      <c r="M146">
+        <v>18.3350568</v>
+      </c>
+      <c r="O146">
+        <v>10.9073959</v>
+      </c>
+      <c r="P146">
+        <v>20.9754309</v>
+      </c>
+      <c r="Q146">
+        <v>17.9560189</v>
+      </c>
+      <c r="R146">
+        <v>12.97533</v>
+      </c>
+      <c r="S146">
+        <v>18.4692339</v>
+      </c>
+      <c r="T146">
+        <v>16.4305433</v>
+      </c>
+      <c r="U146">
+        <v>15.6735795</v>
+      </c>
+      <c r="V146">
+        <v>22.8904417</v>
+      </c>
+      <c r="W146">
+        <v>11.6449151</v>
+      </c>
+      <c r="X146">
+        <v>13.2868916</v>
+      </c>
+      <c r="Y146">
+        <v>9.359681399999999</v>
+      </c>
+      <c r="Z146">
+        <v>10.8732211</v>
+      </c>
+      <c r="AA146">
+        <v>15.0747685</v>
+      </c>
+      <c r="AB146">
+        <v>15.5158109</v>
+      </c>
+      <c r="AD146">
+        <v>24.8879141</v>
+      </c>
+      <c r="AE146">
+        <v>13.1286613</v>
+      </c>
+      <c r="AF146">
+        <v>17.3084322</v>
+      </c>
+      <c r="AG146">
+        <v>16.5407786</v>
+      </c>
+      <c r="AH146">
+        <v>18.2054626</v>
+      </c>
+      <c r="AI146">
+        <v>10.105382</v>
+      </c>
+      <c r="AJ146">
+        <v>12.7694734</v>
+      </c>
+      <c r="AK146">
+        <v>15.3658474</v>
+      </c>
+      <c r="AL146">
+        <v>15.3090244</v>
+      </c>
+      <c r="AM146">
+        <v>12.0433725</v>
+      </c>
+      <c r="AN146">
+        <v>13.181903</v>
+      </c>
+      <c r="AO146">
+        <v>20.2608306</v>
+      </c>
+      <c r="AP146">
+        <v>11.670171</v>
+      </c>
+      <c r="AQ146">
+        <v>11.2953419</v>
+      </c>
+      <c r="AS146">
+        <v>11.2499169</v>
+      </c>
+      <c r="AT146">
+        <v>24.5334944</v>
+      </c>
+      <c r="AU146">
+        <v>20.9010626</v>
+      </c>
+      <c r="AV146">
+        <v>16.1360694</v>
+      </c>
+      <c r="AW146">
+        <v>25.4589453</v>
+      </c>
+      <c r="AX146">
+        <v>20.273411</v>
+      </c>
+      <c r="AY146">
+        <v>13.9455758</v>
+      </c>
+      <c r="BA146">
+        <v>10.5447589</v>
+      </c>
+      <c r="BB146">
+        <v>13.4089693</v>
+      </c>
+      <c r="BC146">
+        <v>13.9999813</v>
+      </c>
+      <c r="BD146">
+        <v>13.6277023</v>
+      </c>
+      <c r="BE146">
+        <v>14.4864613</v>
+      </c>
+    </row>
+    <row r="147" spans="1:57">
+      <c r="A147" t="s">
+        <v>201</v>
+      </c>
+      <c r="B147">
+        <v>16.9937206</v>
+      </c>
+      <c r="C147">
+        <v>23.9362063</v>
+      </c>
+      <c r="D147">
+        <v>21.3845834</v>
+      </c>
+      <c r="F147">
+        <v>26.1843834</v>
+      </c>
+      <c r="G147">
+        <v>13.9620312</v>
+      </c>
+      <c r="H147">
+        <v>12.916085</v>
+      </c>
+      <c r="I147">
+        <v>10.4653022</v>
+      </c>
+      <c r="J147">
+        <v>14.4823067</v>
+      </c>
+      <c r="K147">
+        <v>13.9290012</v>
+      </c>
+      <c r="L147">
+        <v>18.8108153</v>
+      </c>
+      <c r="M147">
+        <v>19.1794568</v>
+      </c>
+      <c r="O147">
+        <v>10.9620419</v>
+      </c>
+      <c r="P147">
+        <v>21.4057367</v>
+      </c>
+      <c r="Q147">
+        <v>18.342754</v>
+      </c>
+      <c r="R147">
+        <v>12.8101213</v>
+      </c>
+      <c r="S147">
+        <v>18.1841856</v>
+      </c>
+      <c r="T147">
+        <v>16.5770114</v>
+      </c>
+      <c r="U147">
+        <v>15.9757011</v>
+      </c>
+      <c r="V147">
+        <v>23.6984248</v>
+      </c>
+      <c r="W147">
+        <v>11.4206894</v>
+      </c>
+      <c r="X147">
+        <v>13.4838192</v>
+      </c>
+      <c r="Y147">
+        <v>10.3614833</v>
+      </c>
+      <c r="Z147">
+        <v>11.2238289</v>
+      </c>
+      <c r="AA147">
+        <v>15.2991228</v>
+      </c>
+      <c r="AB147">
+        <v>16.4231594</v>
+      </c>
+      <c r="AD147">
+        <v>24.2064887</v>
+      </c>
+      <c r="AE147">
+        <v>13.7672723</v>
+      </c>
+      <c r="AF147">
+        <v>17.4648305</v>
+      </c>
+      <c r="AG147">
+        <v>18.0676623</v>
+      </c>
+      <c r="AH147">
+        <v>18.2890104</v>
+      </c>
+      <c r="AI147">
+        <v>9.9858607</v>
+      </c>
+      <c r="AJ147">
+        <v>12.6734429</v>
+      </c>
+      <c r="AK147">
+        <v>15.0338561</v>
+      </c>
+      <c r="AL147">
+        <v>15.7220826</v>
+      </c>
+      <c r="AM147">
+        <v>11.9733308</v>
+      </c>
+      <c r="AN147">
+        <v>13.5822707</v>
+      </c>
+      <c r="AO147">
+        <v>20.8169737</v>
+      </c>
+      <c r="AP147">
+        <v>12.1027921</v>
+      </c>
+      <c r="AQ147">
+        <v>11.3888872</v>
+      </c>
+      <c r="AS147">
+        <v>11.5383538</v>
+      </c>
+      <c r="AT147">
+        <v>25.9422008</v>
+      </c>
+      <c r="AU147">
+        <v>21.1213371</v>
+      </c>
+      <c r="AV147">
+        <v>17.0203399</v>
+      </c>
+      <c r="AW147">
+        <v>26.4850715</v>
+      </c>
+      <c r="AX147">
+        <v>20.9381511</v>
+      </c>
+      <c r="AY147">
+        <v>13.9121521</v>
+      </c>
+      <c r="BA147">
+        <v>10.8428927</v>
+      </c>
+      <c r="BB147">
+        <v>13.3538857</v>
+      </c>
+      <c r="BC147">
+        <v>14.4330377</v>
+      </c>
+      <c r="BD147">
+        <v>13.9714395</v>
+      </c>
+      <c r="BE147">
+        <v>15.4602689</v>
+      </c>
+    </row>
+    <row r="148" spans="1:57">
+      <c r="A148" t="s">
+        <v>202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding data up to 15th
</commit_message>
<xml_diff>
--- a/fb-survey-communityState.xlsx
+++ b/fb-survey-communityState.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="222">
   <si>
     <t>Alaska</t>
   </si>
@@ -656,6 +656,30 @@
   </si>
   <si>
     <t>07 07 2020</t>
+  </si>
+  <si>
+    <t>08 07 2020</t>
+  </si>
+  <si>
+    <t>09 07 2020</t>
+  </si>
+  <si>
+    <t>10 07 2020</t>
+  </si>
+  <si>
+    <t>11 07 2020</t>
+  </si>
+  <si>
+    <t>12 07 2020</t>
+  </si>
+  <si>
+    <t>13 07 2020</t>
+  </si>
+  <si>
+    <t>14 07 2020</t>
+  </si>
+  <si>
+    <t>15 07 2020</t>
   </si>
 </sst>
 </file>
@@ -987,7 +1011,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BE159"/>
+  <dimension ref="A1:BE167"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -12157,6 +12181,9 @@
       <c r="AQ142">
         <v>11.3918073</v>
       </c>
+      <c r="AR142">
+        <v>9.6638655</v>
+      </c>
       <c r="AS142">
         <v>11.8782537</v>
       </c>
@@ -12315,6 +12342,9 @@
       <c r="AQ143">
         <v>11.3086483</v>
       </c>
+      <c r="AR143">
+        <v>14.1026846</v>
+      </c>
       <c r="AS143">
         <v>11.5487716</v>
       </c>
@@ -12473,6 +12503,9 @@
       <c r="AQ144">
         <v>11.3603624</v>
       </c>
+      <c r="AR144">
+        <v>12.5000302</v>
+      </c>
       <c r="AS144">
         <v>10.9600925</v>
       </c>
@@ -12631,6 +12664,9 @@
       <c r="AQ145">
         <v>11.5125593</v>
       </c>
+      <c r="AR145">
+        <v>6.3433735</v>
+      </c>
       <c r="AS145">
         <v>10.8506175</v>
       </c>
@@ -12789,6 +12825,9 @@
       <c r="AQ146">
         <v>11.2953419</v>
       </c>
+      <c r="AR146">
+        <v>9.9206349</v>
+      </c>
       <c r="AS146">
         <v>11.2499169</v>
       </c>
@@ -12947,6 +12986,9 @@
       <c r="AQ147">
         <v>11.3888872</v>
       </c>
+      <c r="AR147">
+        <v>12.3188934</v>
+      </c>
       <c r="AS147">
         <v>11.5383538</v>
       </c>
@@ -14262,7 +14304,7 @@
         <v>23.7480299</v>
       </c>
       <c r="F156">
-        <v>32.4680664</v>
+        <v>32.4653096</v>
       </c>
       <c r="G156">
         <v>17.1070357</v>
@@ -14420,7 +14462,7 @@
         <v>23.3882875</v>
       </c>
       <c r="F157">
-        <v>32.7817647</v>
+        <v>32.7789865</v>
       </c>
       <c r="G157">
         <v>17.3981546</v>
@@ -14459,25 +14501,25 @@
         <v>19.6919228</v>
       </c>
       <c r="T157">
-        <v>20.1720122</v>
+        <v>20.1683719</v>
       </c>
       <c r="U157">
         <v>17.691595</v>
       </c>
       <c r="V157">
-        <v>29.4615414</v>
+        <v>29.4708224</v>
       </c>
       <c r="W157">
         <v>10.8001887</v>
       </c>
       <c r="X157">
-        <v>12.8365451</v>
+        <v>12.8346568</v>
       </c>
       <c r="Y157">
         <v>9.204961900000001</v>
       </c>
       <c r="Z157">
-        <v>12.7940221</v>
+        <v>12.7986214</v>
       </c>
       <c r="AA157">
         <v>16.5790662</v>
@@ -14498,7 +14540,7 @@
         <v>17.9027308</v>
       </c>
       <c r="AH157">
-        <v>21.219769</v>
+        <v>21.213696</v>
       </c>
       <c r="AI157">
         <v>9.691144</v>
@@ -14525,7 +14567,7 @@
         <v>12.8146492</v>
       </c>
       <c r="AQ157">
-        <v>12.4915898</v>
+        <v>12.4952696</v>
       </c>
       <c r="AS157">
         <v>10.7712467</v>
@@ -14540,7 +14582,7 @@
         <v>21.4857692</v>
       </c>
       <c r="AW157">
-        <v>33.7060345</v>
+        <v>33.705177</v>
       </c>
       <c r="AX157">
         <v>25.2997092</v>
@@ -14552,7 +14594,7 @@
         <v>9.669817200000001</v>
       </c>
       <c r="BB157">
-        <v>14.908385</v>
+        <v>14.9071715</v>
       </c>
       <c r="BC157">
         <v>16.8518046</v>
@@ -14568,10 +14610,1427 @@
       <c r="A158" t="s">
         <v>212</v>
       </c>
+      <c r="B158">
+        <v>16.9183253</v>
+      </c>
+      <c r="C158">
+        <v>29.5143513</v>
+      </c>
+      <c r="D158">
+        <v>24.107177</v>
+      </c>
+      <c r="F158">
+        <v>33.3704249</v>
+      </c>
+      <c r="G158">
+        <v>17.6924464</v>
+      </c>
+      <c r="H158">
+        <v>14.8147658</v>
+      </c>
+      <c r="I158">
+        <v>10.2229111</v>
+      </c>
+      <c r="J158">
+        <v>13.9324487</v>
+      </c>
+      <c r="K158">
+        <v>14.7277228</v>
+      </c>
+      <c r="L158">
+        <v>26.3150971</v>
+      </c>
+      <c r="M158">
+        <v>25.6116608</v>
+      </c>
+      <c r="O158">
+        <v>10.7705287</v>
+      </c>
+      <c r="P158">
+        <v>24.528655</v>
+      </c>
+      <c r="Q158">
+        <v>25.3590334</v>
+      </c>
+      <c r="R158">
+        <v>13.4592071</v>
+      </c>
+      <c r="S158">
+        <v>19.9827343</v>
+      </c>
+      <c r="T158">
+        <v>20.4922932</v>
+      </c>
+      <c r="U158">
+        <v>17.6406222</v>
+      </c>
+      <c r="V158">
+        <v>30.1696393</v>
+      </c>
+      <c r="W158">
+        <v>10.475409</v>
+      </c>
+      <c r="X158">
+        <v>13.0648484</v>
+      </c>
+      <c r="Y158">
+        <v>9.9</v>
+      </c>
+      <c r="Z158">
+        <v>13.3700591</v>
+      </c>
+      <c r="AA158">
+        <v>16.4760546</v>
+      </c>
+      <c r="AB158">
+        <v>19.1893983</v>
+      </c>
+      <c r="AD158">
+        <v>28.7638491</v>
+      </c>
+      <c r="AE158">
+        <v>18.4329957</v>
+      </c>
+      <c r="AF158">
+        <v>19.6781178</v>
+      </c>
+      <c r="AG158">
+        <v>19.1976577</v>
+      </c>
+      <c r="AH158">
+        <v>21.2905758</v>
+      </c>
+      <c r="AI158">
+        <v>10.0958565</v>
+      </c>
+      <c r="AJ158">
+        <v>11.642863</v>
+      </c>
+      <c r="AK158">
+        <v>16.4989034</v>
+      </c>
+      <c r="AL158">
+        <v>20.0819124</v>
+      </c>
+      <c r="AM158">
+        <v>10.9822438</v>
+      </c>
+      <c r="AN158">
+        <v>15.9457223</v>
+      </c>
+      <c r="AO158">
+        <v>25.3034962</v>
+      </c>
+      <c r="AP158">
+        <v>12.9228472</v>
+      </c>
+      <c r="AQ158">
+        <v>12.7566773</v>
+      </c>
+      <c r="AS158">
+        <v>10.8671279</v>
+      </c>
+      <c r="AT158">
+        <v>30.1666944</v>
+      </c>
+      <c r="AU158">
+        <v>21.6263594</v>
+      </c>
+      <c r="AV158">
+        <v>21.9745574</v>
+      </c>
+      <c r="AW158">
+        <v>34.1965975</v>
+      </c>
+      <c r="AX158">
+        <v>24.8026304</v>
+      </c>
+      <c r="AY158">
+        <v>15.4307353</v>
+      </c>
+      <c r="BA158">
+        <v>9.700578500000001</v>
+      </c>
+      <c r="BB158">
+        <v>15.4091442</v>
+      </c>
+      <c r="BC158">
+        <v>17.1123663</v>
+      </c>
+      <c r="BD158">
+        <v>17.1643016</v>
+      </c>
+      <c r="BE158">
+        <v>15.8328005</v>
+      </c>
     </row>
     <row r="159" spans="1:57">
       <c r="A159" t="s">
         <v>213</v>
+      </c>
+      <c r="B159">
+        <v>18.540096</v>
+      </c>
+      <c r="C159">
+        <v>30.3507816</v>
+      </c>
+      <c r="D159">
+        <v>23.9970369</v>
+      </c>
+      <c r="F159">
+        <v>33.802515</v>
+      </c>
+      <c r="G159">
+        <v>18.0073822</v>
+      </c>
+      <c r="H159">
+        <v>14.8983356</v>
+      </c>
+      <c r="I159">
+        <v>10.1358924</v>
+      </c>
+      <c r="J159">
+        <v>14.1420118</v>
+      </c>
+      <c r="K159">
+        <v>15.097561</v>
+      </c>
+      <c r="L159">
+        <v>26.7837643</v>
+      </c>
+      <c r="M159">
+        <v>26.2870662</v>
+      </c>
+      <c r="O159">
+        <v>11.3264192</v>
+      </c>
+      <c r="P159">
+        <v>24.9419881</v>
+      </c>
+      <c r="Q159">
+        <v>26.7417414</v>
+      </c>
+      <c r="R159">
+        <v>13.8691768</v>
+      </c>
+      <c r="S159">
+        <v>20.102531</v>
+      </c>
+      <c r="T159">
+        <v>21.5423498</v>
+      </c>
+      <c r="U159">
+        <v>18.6622986</v>
+      </c>
+      <c r="V159">
+        <v>31.2915365</v>
+      </c>
+      <c r="W159">
+        <v>10.4951572</v>
+      </c>
+      <c r="X159">
+        <v>13.3537736</v>
+      </c>
+      <c r="Y159">
+        <v>10.1571114</v>
+      </c>
+      <c r="Z159">
+        <v>13.5461185</v>
+      </c>
+      <c r="AA159">
+        <v>16.5215635</v>
+      </c>
+      <c r="AB159">
+        <v>19.7837845</v>
+      </c>
+      <c r="AD159">
+        <v>29.4474594</v>
+      </c>
+      <c r="AE159">
+        <v>18.7756844</v>
+      </c>
+      <c r="AF159">
+        <v>19.9430736</v>
+      </c>
+      <c r="AG159">
+        <v>18.157946</v>
+      </c>
+      <c r="AH159">
+        <v>21.1176784</v>
+      </c>
+      <c r="AI159">
+        <v>10.3566122</v>
+      </c>
+      <c r="AJ159">
+        <v>11.6876809</v>
+      </c>
+      <c r="AK159">
+        <v>17.1188141</v>
+      </c>
+      <c r="AL159">
+        <v>20.2281426</v>
+      </c>
+      <c r="AM159">
+        <v>11.0039296</v>
+      </c>
+      <c r="AN159">
+        <v>16.387481</v>
+      </c>
+      <c r="AO159">
+        <v>25.547398</v>
+      </c>
+      <c r="AP159">
+        <v>13.2311248</v>
+      </c>
+      <c r="AQ159">
+        <v>12.6931724</v>
+      </c>
+      <c r="AS159">
+        <v>10.8970687</v>
+      </c>
+      <c r="AT159">
+        <v>30.105139</v>
+      </c>
+      <c r="AU159">
+        <v>21.9915205</v>
+      </c>
+      <c r="AV159">
+        <v>22.8504615</v>
+      </c>
+      <c r="AW159">
+        <v>34.7858815</v>
+      </c>
+      <c r="AX159">
+        <v>25.0153675</v>
+      </c>
+      <c r="AY159">
+        <v>15.6163363</v>
+      </c>
+      <c r="BA159">
+        <v>8.601823</v>
+      </c>
+      <c r="BB159">
+        <v>15.7853958</v>
+      </c>
+      <c r="BC159">
+        <v>17.3608334</v>
+      </c>
+      <c r="BD159">
+        <v>17.542068</v>
+      </c>
+      <c r="BE159">
+        <v>16.6247329</v>
+      </c>
+    </row>
+    <row r="160" spans="1:57">
+      <c r="A160" t="s">
+        <v>214</v>
+      </c>
+      <c r="B160">
+        <v>18.197634</v>
+      </c>
+      <c r="C160">
+        <v>31.4844674</v>
+      </c>
+      <c r="D160">
+        <v>24.0797015</v>
+      </c>
+      <c r="F160">
+        <v>33.7000066</v>
+      </c>
+      <c r="G160">
+        <v>18.5504864</v>
+      </c>
+      <c r="H160">
+        <v>15.3646456</v>
+      </c>
+      <c r="I160">
+        <v>9.551384499999999</v>
+      </c>
+      <c r="J160">
+        <v>14.0423032</v>
+      </c>
+      <c r="K160">
+        <v>15.4932735</v>
+      </c>
+      <c r="L160">
+        <v>27.3962847</v>
+      </c>
+      <c r="M160">
+        <v>27.3502762</v>
+      </c>
+      <c r="O160">
+        <v>10.3878116</v>
+      </c>
+      <c r="P160">
+        <v>25.839906</v>
+      </c>
+      <c r="Q160">
+        <v>27.6209115</v>
+      </c>
+      <c r="R160">
+        <v>14.2405344</v>
+      </c>
+      <c r="S160">
+        <v>20.382524</v>
+      </c>
+      <c r="T160">
+        <v>21.9070784</v>
+      </c>
+      <c r="U160">
+        <v>18.5532281</v>
+      </c>
+      <c r="V160">
+        <v>31.7126262</v>
+      </c>
+      <c r="W160">
+        <v>10.5243153</v>
+      </c>
+      <c r="X160">
+        <v>13.2871455</v>
+      </c>
+      <c r="Y160">
+        <v>9.926656599999999</v>
+      </c>
+      <c r="Z160">
+        <v>13.7146305</v>
+      </c>
+      <c r="AA160">
+        <v>17.0930184</v>
+      </c>
+      <c r="AB160">
+        <v>19.7885177</v>
+      </c>
+      <c r="AD160">
+        <v>30.3346846</v>
+      </c>
+      <c r="AE160">
+        <v>19.7161342</v>
+      </c>
+      <c r="AF160">
+        <v>19.992823</v>
+      </c>
+      <c r="AG160">
+        <v>18.6846111</v>
+      </c>
+      <c r="AH160">
+        <v>21.4337795</v>
+      </c>
+      <c r="AI160">
+        <v>10.2089805</v>
+      </c>
+      <c r="AJ160">
+        <v>11.7189474</v>
+      </c>
+      <c r="AK160">
+        <v>17.1653453</v>
+      </c>
+      <c r="AL160">
+        <v>21.2486593</v>
+      </c>
+      <c r="AM160">
+        <v>11.1026743</v>
+      </c>
+      <c r="AN160">
+        <v>16.6487976</v>
+      </c>
+      <c r="AO160">
+        <v>26.3150892</v>
+      </c>
+      <c r="AP160">
+        <v>13.8597935</v>
+      </c>
+      <c r="AQ160">
+        <v>12.9421702</v>
+      </c>
+      <c r="AS160">
+        <v>11.1516148</v>
+      </c>
+      <c r="AT160">
+        <v>30.6113227</v>
+      </c>
+      <c r="AU160">
+        <v>21.1885529</v>
+      </c>
+      <c r="AV160">
+        <v>23.4921564</v>
+      </c>
+      <c r="AW160">
+        <v>34.9544485</v>
+      </c>
+      <c r="AX160">
+        <v>25.3308189</v>
+      </c>
+      <c r="AY160">
+        <v>16.1464001</v>
+      </c>
+      <c r="BA160">
+        <v>9.5851764</v>
+      </c>
+      <c r="BB160">
+        <v>16.2511838</v>
+      </c>
+      <c r="BC160">
+        <v>17.4881269</v>
+      </c>
+      <c r="BD160">
+        <v>17.8434843</v>
+      </c>
+      <c r="BE160">
+        <v>16.8749846</v>
+      </c>
+    </row>
+    <row r="161" spans="1:57">
+      <c r="A161" t="s">
+        <v>215</v>
+      </c>
+      <c r="B161">
+        <v>19.7042641</v>
+      </c>
+      <c r="C161">
+        <v>32.5005568</v>
+      </c>
+      <c r="D161">
+        <v>24.4717329</v>
+      </c>
+      <c r="F161">
+        <v>33.663415</v>
+      </c>
+      <c r="G161">
+        <v>18.890091</v>
+      </c>
+      <c r="H161">
+        <v>15.5951172</v>
+      </c>
+      <c r="I161">
+        <v>9.735512999999999</v>
+      </c>
+      <c r="J161">
+        <v>14.5314353</v>
+      </c>
+      <c r="K161">
+        <v>15.7330652</v>
+      </c>
+      <c r="L161">
+        <v>27.6561341</v>
+      </c>
+      <c r="M161">
+        <v>28.3518815</v>
+      </c>
+      <c r="O161">
+        <v>10.5304212</v>
+      </c>
+      <c r="P161">
+        <v>26.249919</v>
+      </c>
+      <c r="Q161">
+        <v>27.8090574</v>
+      </c>
+      <c r="R161">
+        <v>14.8367973</v>
+      </c>
+      <c r="S161">
+        <v>21.1088812</v>
+      </c>
+      <c r="T161">
+        <v>22.8405003</v>
+      </c>
+      <c r="U161">
+        <v>18.8234783</v>
+      </c>
+      <c r="V161">
+        <v>32.50586</v>
+      </c>
+      <c r="W161">
+        <v>10.8127532</v>
+      </c>
+      <c r="X161">
+        <v>13.6640493</v>
+      </c>
+      <c r="Y161">
+        <v>10.6006583</v>
+      </c>
+      <c r="Z161">
+        <v>14.2797998</v>
+      </c>
+      <c r="AA161">
+        <v>17.2841197</v>
+      </c>
+      <c r="AB161">
+        <v>20.654161</v>
+      </c>
+      <c r="AD161">
+        <v>30.5350005</v>
+      </c>
+      <c r="AE161">
+        <v>19.9262169</v>
+      </c>
+      <c r="AF161">
+        <v>20.2679215</v>
+      </c>
+      <c r="AG161">
+        <v>18.5492036</v>
+      </c>
+      <c r="AH161">
+        <v>21.4314004</v>
+      </c>
+      <c r="AI161">
+        <v>10.5608046</v>
+      </c>
+      <c r="AJ161">
+        <v>11.7918518</v>
+      </c>
+      <c r="AK161">
+        <v>16.8835545</v>
+      </c>
+      <c r="AL161">
+        <v>21.3683338</v>
+      </c>
+      <c r="AM161">
+        <v>11.3579482</v>
+      </c>
+      <c r="AN161">
+        <v>16.8949676</v>
+      </c>
+      <c r="AO161">
+        <v>26.9110247</v>
+      </c>
+      <c r="AP161">
+        <v>14.3032515</v>
+      </c>
+      <c r="AQ161">
+        <v>13.2085646</v>
+      </c>
+      <c r="AS161">
+        <v>11.7751507</v>
+      </c>
+      <c r="AT161">
+        <v>30.9650017</v>
+      </c>
+      <c r="AU161">
+        <v>22.6290361</v>
+      </c>
+      <c r="AV161">
+        <v>24.1840717</v>
+      </c>
+      <c r="AW161">
+        <v>35.6002134</v>
+      </c>
+      <c r="AX161">
+        <v>25.122235</v>
+      </c>
+      <c r="AY161">
+        <v>16.1649252</v>
+      </c>
+      <c r="BA161">
+        <v>8.5948767</v>
+      </c>
+      <c r="BB161">
+        <v>16.4536366</v>
+      </c>
+      <c r="BC161">
+        <v>18.0352443</v>
+      </c>
+      <c r="BD161">
+        <v>18.0270042</v>
+      </c>
+      <c r="BE161">
+        <v>17.4189924</v>
+      </c>
+    </row>
+    <row r="162" spans="1:57">
+      <c r="A162" t="s">
+        <v>216</v>
+      </c>
+      <c r="B162">
+        <v>20.382372</v>
+      </c>
+      <c r="C162">
+        <v>32.4618765</v>
+      </c>
+      <c r="D162">
+        <v>24.6116366</v>
+      </c>
+      <c r="F162">
+        <v>34.0362763</v>
+      </c>
+      <c r="G162">
+        <v>19.1068955</v>
+      </c>
+      <c r="H162">
+        <v>15.9813237</v>
+      </c>
+      <c r="I162">
+        <v>9.470913100000001</v>
+      </c>
+      <c r="J162">
+        <v>14.0736342</v>
+      </c>
+      <c r="K162">
+        <v>15.7998252</v>
+      </c>
+      <c r="L162">
+        <v>28.0292812</v>
+      </c>
+      <c r="M162">
+        <v>29.2316447</v>
+      </c>
+      <c r="O162">
+        <v>10.6965174</v>
+      </c>
+      <c r="P162">
+        <v>26.3172584</v>
+      </c>
+      <c r="Q162">
+        <v>28.055521</v>
+      </c>
+      <c r="R162">
+        <v>15.4020479</v>
+      </c>
+      <c r="S162">
+        <v>21.6407044</v>
+      </c>
+      <c r="T162">
+        <v>23.6480803</v>
+      </c>
+      <c r="U162">
+        <v>19.2725137</v>
+      </c>
+      <c r="V162">
+        <v>33.4794689</v>
+      </c>
+      <c r="W162">
+        <v>10.99812</v>
+      </c>
+      <c r="X162">
+        <v>13.6256903</v>
+      </c>
+      <c r="Y162">
+        <v>10.2540355</v>
+      </c>
+      <c r="Z162">
+        <v>14.5724986</v>
+      </c>
+      <c r="AA162">
+        <v>17.7304814</v>
+      </c>
+      <c r="AB162">
+        <v>20.9043963</v>
+      </c>
+      <c r="AD162">
+        <v>31.3898123</v>
+      </c>
+      <c r="AE162">
+        <v>18.7238945</v>
+      </c>
+      <c r="AF162">
+        <v>20.2710843</v>
+      </c>
+      <c r="AG162">
+        <v>20.8673608</v>
+      </c>
+      <c r="AH162">
+        <v>21.6024612</v>
+      </c>
+      <c r="AI162">
+        <v>10.4267425</v>
+      </c>
+      <c r="AJ162">
+        <v>11.7741789</v>
+      </c>
+      <c r="AK162">
+        <v>17.3505791</v>
+      </c>
+      <c r="AL162">
+        <v>22.5339997</v>
+      </c>
+      <c r="AM162">
+        <v>11.5262973</v>
+      </c>
+      <c r="AN162">
+        <v>17.1613543</v>
+      </c>
+      <c r="AO162">
+        <v>27.7904621</v>
+      </c>
+      <c r="AP162">
+        <v>14.2139927</v>
+      </c>
+      <c r="AQ162">
+        <v>13.6003307</v>
+      </c>
+      <c r="AS162">
+        <v>11.6738569</v>
+      </c>
+      <c r="AT162">
+        <v>31.6753206</v>
+      </c>
+      <c r="AU162">
+        <v>22.6671</v>
+      </c>
+      <c r="AV162">
+        <v>24.630052</v>
+      </c>
+      <c r="AW162">
+        <v>36.0287863</v>
+      </c>
+      <c r="AX162">
+        <v>25.8646409</v>
+      </c>
+      <c r="AY162">
+        <v>16.479992</v>
+      </c>
+      <c r="BA162">
+        <v>8.480681499999999</v>
+      </c>
+      <c r="BB162">
+        <v>16.9239729</v>
+      </c>
+      <c r="BC162">
+        <v>18.8778053</v>
+      </c>
+      <c r="BD162">
+        <v>18.4857864</v>
+      </c>
+      <c r="BE162">
+        <v>19.0715124</v>
+      </c>
+    </row>
+    <row r="163" spans="1:57">
+      <c r="A163" t="s">
+        <v>217</v>
+      </c>
+      <c r="B163">
+        <v>20.1459391</v>
+      </c>
+      <c r="C163">
+        <v>33.1856147</v>
+      </c>
+      <c r="D163">
+        <v>24.9718846</v>
+      </c>
+      <c r="F163">
+        <v>33.675882</v>
+      </c>
+      <c r="G163">
+        <v>19.5523072</v>
+      </c>
+      <c r="H163">
+        <v>16.1401716</v>
+      </c>
+      <c r="I163">
+        <v>9.980370499999999</v>
+      </c>
+      <c r="J163">
+        <v>14.0642939</v>
+      </c>
+      <c r="K163">
+        <v>16.0867698</v>
+      </c>
+      <c r="L163">
+        <v>28.4399577</v>
+      </c>
+      <c r="M163">
+        <v>29.8730243</v>
+      </c>
+      <c r="O163">
+        <v>11.0353535</v>
+      </c>
+      <c r="P163">
+        <v>26.8472813</v>
+      </c>
+      <c r="Q163">
+        <v>28.4823756</v>
+      </c>
+      <c r="R163">
+        <v>15.9794238</v>
+      </c>
+      <c r="S163">
+        <v>21.5582374</v>
+      </c>
+      <c r="T163">
+        <v>23.9433336</v>
+      </c>
+      <c r="U163">
+        <v>19.3815299</v>
+      </c>
+      <c r="V163">
+        <v>33.7468987</v>
+      </c>
+      <c r="W163">
+        <v>10.8430414</v>
+      </c>
+      <c r="X163">
+        <v>13.7605188</v>
+      </c>
+      <c r="Y163">
+        <v>10.3998961</v>
+      </c>
+      <c r="Z163">
+        <v>14.7176725</v>
+      </c>
+      <c r="AA163">
+        <v>18.0537978</v>
+      </c>
+      <c r="AB163">
+        <v>21.2060415</v>
+      </c>
+      <c r="AD163">
+        <v>31.7221948</v>
+      </c>
+      <c r="AE163">
+        <v>19.8526649</v>
+      </c>
+      <c r="AF163">
+        <v>20.4488728</v>
+      </c>
+      <c r="AG163">
+        <v>19.7551759</v>
+      </c>
+      <c r="AH163">
+        <v>21.710834</v>
+      </c>
+      <c r="AI163">
+        <v>10.1017042</v>
+      </c>
+      <c r="AJ163">
+        <v>11.8543623</v>
+      </c>
+      <c r="AK163">
+        <v>17.7799838</v>
+      </c>
+      <c r="AL163">
+        <v>23.3497166</v>
+      </c>
+      <c r="AM163">
+        <v>11.7677035</v>
+      </c>
+      <c r="AN163">
+        <v>17.6238576</v>
+      </c>
+      <c r="AO163">
+        <v>27.6707333</v>
+      </c>
+      <c r="AP163">
+        <v>14.5636303</v>
+      </c>
+      <c r="AQ163">
+        <v>13.675631</v>
+      </c>
+      <c r="AS163">
+        <v>11.8656667</v>
+      </c>
+      <c r="AT163">
+        <v>31.8462533</v>
+      </c>
+      <c r="AU163">
+        <v>23.1889159</v>
+      </c>
+      <c r="AV163">
+        <v>24.8443858</v>
+      </c>
+      <c r="AW163">
+        <v>36.6818059</v>
+      </c>
+      <c r="AX163">
+        <v>25.6927497</v>
+      </c>
+      <c r="AY163">
+        <v>16.6324797</v>
+      </c>
+      <c r="BA163">
+        <v>9.6381801</v>
+      </c>
+      <c r="BB163">
+        <v>17.0988719</v>
+      </c>
+      <c r="BC163">
+        <v>19.4696877</v>
+      </c>
+      <c r="BD163">
+        <v>18.5877909</v>
+      </c>
+      <c r="BE163">
+        <v>19.2370293</v>
+      </c>
+    </row>
+    <row r="164" spans="1:57">
+      <c r="A164" t="s">
+        <v>218</v>
+      </c>
+      <c r="B164">
+        <v>21.0140306</v>
+      </c>
+      <c r="C164">
+        <v>33.6131484</v>
+      </c>
+      <c r="D164">
+        <v>25.1359934</v>
+      </c>
+      <c r="F164">
+        <v>34.0000635</v>
+      </c>
+      <c r="G164">
+        <v>19.8873091</v>
+      </c>
+      <c r="H164">
+        <v>16.1697976</v>
+      </c>
+      <c r="I164">
+        <v>9.966300499999999</v>
+      </c>
+      <c r="J164">
+        <v>13.396861</v>
+      </c>
+      <c r="K164">
+        <v>16.8050699</v>
+      </c>
+      <c r="L164">
+        <v>28.7717943</v>
+      </c>
+      <c r="M164">
+        <v>30.6282619</v>
+      </c>
+      <c r="O164">
+        <v>11.1602497</v>
+      </c>
+      <c r="P164">
+        <v>27.3507073</v>
+      </c>
+      <c r="Q164">
+        <v>29.102253</v>
+      </c>
+      <c r="R164">
+        <v>16.2861879</v>
+      </c>
+      <c r="S164">
+        <v>22.1573037</v>
+      </c>
+      <c r="T164">
+        <v>24.7486555</v>
+      </c>
+      <c r="U164">
+        <v>20.0155098</v>
+      </c>
+      <c r="V164">
+        <v>34.0333781</v>
+      </c>
+      <c r="W164">
+        <v>11.041463</v>
+      </c>
+      <c r="X164">
+        <v>14.2828296</v>
+      </c>
+      <c r="Y164">
+        <v>10.9900457</v>
+      </c>
+      <c r="Z164">
+        <v>15.0396092</v>
+      </c>
+      <c r="AA164">
+        <v>18.4962669</v>
+      </c>
+      <c r="AB164">
+        <v>21.8253941</v>
+      </c>
+      <c r="AD164">
+        <v>33.1677202</v>
+      </c>
+      <c r="AE164">
+        <v>19.2988576</v>
+      </c>
+      <c r="AF164">
+        <v>20.6208636</v>
+      </c>
+      <c r="AG164">
+        <v>21.0689236</v>
+      </c>
+      <c r="AH164">
+        <v>21.7470439</v>
+      </c>
+      <c r="AI164">
+        <v>10.2026457</v>
+      </c>
+      <c r="AJ164">
+        <v>11.8747435</v>
+      </c>
+      <c r="AK164">
+        <v>17.6386579</v>
+      </c>
+      <c r="AL164">
+        <v>23.367593</v>
+      </c>
+      <c r="AM164">
+        <v>11.9330541</v>
+      </c>
+      <c r="AN164">
+        <v>18.3314672</v>
+      </c>
+      <c r="AO164">
+        <v>27.9180883</v>
+      </c>
+      <c r="AP164">
+        <v>15.0514105</v>
+      </c>
+      <c r="AQ164">
+        <v>13.736239</v>
+      </c>
+      <c r="AS164">
+        <v>11.389702</v>
+      </c>
+      <c r="AT164">
+        <v>32.2731426</v>
+      </c>
+      <c r="AU164">
+        <v>23.2163726</v>
+      </c>
+      <c r="AV164">
+        <v>25.7752316</v>
+      </c>
+      <c r="AW164">
+        <v>36.8295252</v>
+      </c>
+      <c r="AX164">
+        <v>26.2702635</v>
+      </c>
+      <c r="AY164">
+        <v>16.906638</v>
+      </c>
+      <c r="BA164">
+        <v>8.4644455</v>
+      </c>
+      <c r="BB164">
+        <v>16.9925478</v>
+      </c>
+      <c r="BC164">
+        <v>19.5397754</v>
+      </c>
+      <c r="BD164">
+        <v>19.4989579</v>
+      </c>
+      <c r="BE164">
+        <v>19.7099731</v>
+      </c>
+    </row>
+    <row r="165" spans="1:57">
+      <c r="A165" t="s">
+        <v>219</v>
+      </c>
+      <c r="B165">
+        <v>21.0707577</v>
+      </c>
+      <c r="C165">
+        <v>35.0592101</v>
+      </c>
+      <c r="D165">
+        <v>25.6044353</v>
+      </c>
+      <c r="F165">
+        <v>33.9178388</v>
+      </c>
+      <c r="G165">
+        <v>20.1835229</v>
+      </c>
+      <c r="H165">
+        <v>16.2827761</v>
+      </c>
+      <c r="I165">
+        <v>10.2342095</v>
+      </c>
+      <c r="J165">
+        <v>12.962963</v>
+      </c>
+      <c r="K165">
+        <v>16.7743325</v>
+      </c>
+      <c r="L165">
+        <v>29.3247194</v>
+      </c>
+      <c r="M165">
+        <v>31.2932619</v>
+      </c>
+      <c r="O165">
+        <v>11.316568</v>
+      </c>
+      <c r="P165">
+        <v>27.87526</v>
+      </c>
+      <c r="Q165">
+        <v>30.4004959</v>
+      </c>
+      <c r="R165">
+        <v>16.674027</v>
+      </c>
+      <c r="S165">
+        <v>22.1782766</v>
+      </c>
+      <c r="T165">
+        <v>25.2930529</v>
+      </c>
+      <c r="U165">
+        <v>20.4806406</v>
+      </c>
+      <c r="V165">
+        <v>34.3886942</v>
+      </c>
+      <c r="W165">
+        <v>11.0236526</v>
+      </c>
+      <c r="X165">
+        <v>14.2162917</v>
+      </c>
+      <c r="Y165">
+        <v>10.8833242</v>
+      </c>
+      <c r="Z165">
+        <v>15.0813544</v>
+      </c>
+      <c r="AA165">
+        <v>19.2787578</v>
+      </c>
+      <c r="AB165">
+        <v>22.2925693</v>
+      </c>
+      <c r="AD165">
+        <v>33.0277497</v>
+      </c>
+      <c r="AE165">
+        <v>20.0907005</v>
+      </c>
+      <c r="AF165">
+        <v>20.6148735</v>
+      </c>
+      <c r="AG165">
+        <v>21.0551163</v>
+      </c>
+      <c r="AH165">
+        <v>22.4085361</v>
+      </c>
+      <c r="AI165">
+        <v>10.3627672</v>
+      </c>
+      <c r="AJ165">
+        <v>11.8702682</v>
+      </c>
+      <c r="AK165">
+        <v>17.8907546</v>
+      </c>
+      <c r="AL165">
+        <v>24.1088139</v>
+      </c>
+      <c r="AM165">
+        <v>11.8892303</v>
+      </c>
+      <c r="AN165">
+        <v>18.677243</v>
+      </c>
+      <c r="AO165">
+        <v>27.9416774</v>
+      </c>
+      <c r="AP165">
+        <v>15.2937178</v>
+      </c>
+      <c r="AQ165">
+        <v>13.8130742</v>
+      </c>
+      <c r="AS165">
+        <v>11.4429624</v>
+      </c>
+      <c r="AT165">
+        <v>32.4104225</v>
+      </c>
+      <c r="AU165">
+        <v>22.8237693</v>
+      </c>
+      <c r="AV165">
+        <v>26.2592025</v>
+      </c>
+      <c r="AW165">
+        <v>36.5479858</v>
+      </c>
+      <c r="AX165">
+        <v>27.3497737</v>
+      </c>
+      <c r="AY165">
+        <v>17.3724394</v>
+      </c>
+      <c r="BA165">
+        <v>8.964498799999999</v>
+      </c>
+      <c r="BB165">
+        <v>17.1777709</v>
+      </c>
+      <c r="BC165">
+        <v>20.1971216</v>
+      </c>
+      <c r="BD165">
+        <v>19.1533166</v>
+      </c>
+      <c r="BE165">
+        <v>19.6826186</v>
+      </c>
+    </row>
+    <row r="166" spans="1:57">
+      <c r="A166" t="s">
+        <v>220</v>
+      </c>
+      <c r="B166">
+        <v>21.1761121</v>
+      </c>
+      <c r="C166">
+        <v>35.4318376</v>
+      </c>
+      <c r="D166">
+        <v>25.7271968</v>
+      </c>
+      <c r="F166">
+        <v>33.7522053</v>
+      </c>
+      <c r="G166">
+        <v>20.4414942</v>
+      </c>
+      <c r="H166">
+        <v>16.6002548</v>
+      </c>
+      <c r="I166">
+        <v>10.3587963</v>
+      </c>
+      <c r="J166">
+        <v>13.368669</v>
+      </c>
+      <c r="K166">
+        <v>17.0693028</v>
+      </c>
+      <c r="L166">
+        <v>29.6575934</v>
+      </c>
+      <c r="M166">
+        <v>31.6967999</v>
+      </c>
+      <c r="O166">
+        <v>11.3525391</v>
+      </c>
+      <c r="P166">
+        <v>27.8229325</v>
+      </c>
+      <c r="Q166">
+        <v>31.2854616</v>
+      </c>
+      <c r="R166">
+        <v>16.8814154</v>
+      </c>
+      <c r="S166">
+        <v>22.7565397</v>
+      </c>
+      <c r="T166">
+        <v>25.4999925</v>
+      </c>
+      <c r="U166">
+        <v>20.702807</v>
+      </c>
+      <c r="V166">
+        <v>34.0504716</v>
+      </c>
+      <c r="W166">
+        <v>11.1837746</v>
+      </c>
+      <c r="X166">
+        <v>14.251715</v>
+      </c>
+      <c r="Y166">
+        <v>10.543989</v>
+      </c>
+      <c r="Z166">
+        <v>15.2867517</v>
+      </c>
+      <c r="AA166">
+        <v>19.2937183</v>
+      </c>
+      <c r="AB166">
+        <v>22.1773134</v>
+      </c>
+      <c r="AD166">
+        <v>33.6324745</v>
+      </c>
+      <c r="AE166">
+        <v>19.8004753</v>
+      </c>
+      <c r="AF166">
+        <v>21.0336649</v>
+      </c>
+      <c r="AG166">
+        <v>20.937093</v>
+      </c>
+      <c r="AH166">
+        <v>22.4269818</v>
+      </c>
+      <c r="AI166">
+        <v>10.1571899</v>
+      </c>
+      <c r="AJ166">
+        <v>12.2255893</v>
+      </c>
+      <c r="AK166">
+        <v>18.6536533</v>
+      </c>
+      <c r="AL166">
+        <v>24.0143003</v>
+      </c>
+      <c r="AM166">
+        <v>11.6886585</v>
+      </c>
+      <c r="AN166">
+        <v>19.1965769</v>
+      </c>
+      <c r="AO166">
+        <v>28.1369815</v>
+      </c>
+      <c r="AP166">
+        <v>15.0680596</v>
+      </c>
+      <c r="AQ166">
+        <v>14.0810271</v>
+      </c>
+      <c r="AS166">
+        <v>11.2094101</v>
+      </c>
+      <c r="AT166">
+        <v>32.7838938</v>
+      </c>
+      <c r="AU166">
+        <v>24.5317403</v>
+      </c>
+      <c r="AV166">
+        <v>26.5720371</v>
+      </c>
+      <c r="AW166">
+        <v>36.6617892</v>
+      </c>
+      <c r="AX166">
+        <v>26.8216569</v>
+      </c>
+      <c r="AY166">
+        <v>17.6626752</v>
+      </c>
+      <c r="BA166">
+        <v>8.6423404</v>
+      </c>
+      <c r="BB166">
+        <v>17.3735058</v>
+      </c>
+      <c r="BC166">
+        <v>20.3850363</v>
+      </c>
+      <c r="BD166">
+        <v>19.1470154</v>
+      </c>
+      <c r="BE166">
+        <v>20.4452796</v>
+      </c>
+    </row>
+    <row r="167" spans="1:57">
+      <c r="A167" t="s">
+        <v>221</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data up to 7th second
</commit_message>
<xml_diff>
--- a/fb-survey-communityState.xlsx
+++ b/fb-survey-communityState.xlsx
@@ -24555,7 +24555,7 @@
         <v>12.3646961</v>
       </c>
       <c r="L219">
-        <v>19.6124014</v>
+        <v>19.6167959</v>
       </c>
       <c r="M219">
         <v>26.3352541</v>
@@ -24630,7 +24630,7 @@
         <v>18.8131006</v>
       </c>
       <c r="AM219">
-        <v>10.484613</v>
+        <v>10.4909178</v>
       </c>
       <c r="AN219">
         <v>17.6314449</v>
@@ -24669,7 +24669,7 @@
         <v>8.9175927</v>
       </c>
       <c r="BB219">
-        <v>15.0696204</v>
+        <v>15.0676587</v>
       </c>
       <c r="BC219">
         <v>19.8449583</v>
@@ -24684,6 +24684,159 @@
     <row r="220" spans="1:57">
       <c r="A220" t="s">
         <v>274</v>
+      </c>
+      <c r="B220">
+        <v>19.348659</v>
+      </c>
+      <c r="C220">
+        <v>28.1589014</v>
+      </c>
+      <c r="D220">
+        <v>27.1531579</v>
+      </c>
+      <c r="F220">
+        <v>17.0568446</v>
+      </c>
+      <c r="G220">
+        <v>15.1358517</v>
+      </c>
+      <c r="H220">
+        <v>15.4303285</v>
+      </c>
+      <c r="I220">
+        <v>9.4494962</v>
+      </c>
+      <c r="J220">
+        <v>12.7850163</v>
+      </c>
+      <c r="K220">
+        <v>12.1351126</v>
+      </c>
+      <c r="L220">
+        <v>19.4098882</v>
+      </c>
+      <c r="M220">
+        <v>26.6449402</v>
+      </c>
+      <c r="O220">
+        <v>15.2122642</v>
+      </c>
+      <c r="P220">
+        <v>30.8076175</v>
+      </c>
+      <c r="Q220">
+        <v>26.8548524</v>
+      </c>
+      <c r="R220">
+        <v>20.3163569</v>
+      </c>
+      <c r="S220">
+        <v>25.2872618</v>
+      </c>
+      <c r="T220">
+        <v>26.2278085</v>
+      </c>
+      <c r="U220">
+        <v>23.8883276</v>
+      </c>
+      <c r="V220">
+        <v>24.0808368</v>
+      </c>
+      <c r="W220">
+        <v>10.572511</v>
+      </c>
+      <c r="X220">
+        <v>13.2732579</v>
+      </c>
+      <c r="Y220">
+        <v>10.2195504</v>
+      </c>
+      <c r="Z220">
+        <v>14.713122</v>
+      </c>
+      <c r="AA220">
+        <v>17.4347372</v>
+      </c>
+      <c r="AB220">
+        <v>28.3327067</v>
+      </c>
+      <c r="AD220">
+        <v>29.4071465</v>
+      </c>
+      <c r="AE220">
+        <v>21.4139167</v>
+      </c>
+      <c r="AF220">
+        <v>18.6057406</v>
+      </c>
+      <c r="AG220">
+        <v>30.4878895</v>
+      </c>
+      <c r="AH220">
+        <v>27.5223972</v>
+      </c>
+      <c r="AI220">
+        <v>10.190577</v>
+      </c>
+      <c r="AJ220">
+        <v>10.2358082</v>
+      </c>
+      <c r="AK220">
+        <v>15.2640431</v>
+      </c>
+      <c r="AL220">
+        <v>19.4593548</v>
+      </c>
+      <c r="AM220">
+        <v>10.6828715</v>
+      </c>
+      <c r="AN220">
+        <v>17.6952049</v>
+      </c>
+      <c r="AO220">
+        <v>28.0529212</v>
+      </c>
+      <c r="AP220">
+        <v>12.8612298</v>
+      </c>
+      <c r="AQ220">
+        <v>13.473985</v>
+      </c>
+      <c r="AS220">
+        <v>11.1259162</v>
+      </c>
+      <c r="AT220">
+        <v>21.8564621</v>
+      </c>
+      <c r="AU220">
+        <v>33.5761595</v>
+      </c>
+      <c r="AV220">
+        <v>26.6859001</v>
+      </c>
+      <c r="AW220">
+        <v>21.7190371</v>
+      </c>
+      <c r="AX220">
+        <v>23.0825918</v>
+      </c>
+      <c r="AY220">
+        <v>17.4920161</v>
+      </c>
+      <c r="BA220">
+        <v>8.7037075</v>
+      </c>
+      <c r="BB220">
+        <v>15.0425407</v>
+      </c>
+      <c r="BC220">
+        <v>19.829063</v>
+      </c>
+      <c r="BD220">
+        <v>20.1521553</v>
+      </c>
+      <c r="BE220">
+        <v>19.6242761</v>
       </c>
     </row>
     <row r="221" spans="1:57">

</xml_diff>